<commit_message>
Added several Q3 journals
</commit_message>
<xml_diff>
--- a/source/Journals.xlsx
+++ b/source/Journals.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="530">
   <si>
     <t>Journal</t>
   </si>
@@ -911,7 +911,7 @@
     <t>Foundations and Trends® in Machine Learning</t>
   </si>
   <si>
-    <t>$860</t>
+    <t>860 EUR</t>
   </si>
   <si>
     <t>https://www.nowpublishers.com/MAL</t>
@@ -1955,6 +1955,18 @@
   </si>
   <si>
     <t>Ревью за 4 недели (+50 USD)</t>
+  </si>
+  <si>
+    <t>International Journal of Computational Science and Engineering</t>
+  </si>
+  <si>
+    <t>https://www.scimagojr.com/journalsearch.php?q=6100152804&amp;tip=sid</t>
+  </si>
+  <si>
+    <t>https://www.inderscience.com/info/inarticle.php?artid=107348</t>
+  </si>
+  <si>
+    <t>Второй источник статей</t>
   </si>
   <si>
     <t>Conference</t>
@@ -4035,7 +4047,7 @@
       <c r="B56" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="24" t="s">
         <v>229</v>
       </c>
       <c r="D56" s="10" t="s">
@@ -14203,140 +14215,141 @@
     <hyperlink r:id="rId111" ref="D55"/>
     <hyperlink r:id="rId112" ref="E55"/>
     <hyperlink r:id="rId113" ref="F55"/>
-    <hyperlink r:id="rId114" ref="D56"/>
-    <hyperlink r:id="rId115" ref="D57"/>
-    <hyperlink r:id="rId116" ref="E57"/>
-    <hyperlink r:id="rId117" location="1069-2509" ref="C58"/>
-    <hyperlink r:id="rId118" location="open-access" ref="D58"/>
-    <hyperlink r:id="rId119" location="1069-2509" ref="F58"/>
-    <hyperlink r:id="rId120" ref="C59"/>
-    <hyperlink r:id="rId121" ref="D59"/>
-    <hyperlink r:id="rId122" ref="E59"/>
-    <hyperlink r:id="rId123" ref="D60"/>
-    <hyperlink r:id="rId124" ref="E60"/>
-    <hyperlink r:id="rId125" ref="D61"/>
-    <hyperlink r:id="rId126" ref="E61"/>
-    <hyperlink r:id="rId127" ref="C62"/>
-    <hyperlink r:id="rId128" ref="D62"/>
-    <hyperlink r:id="rId129" location="Fees%20and%20funding" ref="C63"/>
-    <hyperlink r:id="rId130" ref="D63"/>
-    <hyperlink r:id="rId131" ref="E63"/>
-    <hyperlink r:id="rId132" ref="C64"/>
-    <hyperlink r:id="rId133" ref="D64"/>
-    <hyperlink r:id="rId134" ref="E64"/>
-    <hyperlink r:id="rId135" ref="F64"/>
-    <hyperlink r:id="rId136" ref="C65"/>
-    <hyperlink r:id="rId137" ref="D65"/>
-    <hyperlink r:id="rId138" ref="D66"/>
-    <hyperlink r:id="rId139" ref="E66"/>
-    <hyperlink r:id="rId140" ref="C67"/>
-    <hyperlink r:id="rId141" ref="D67"/>
-    <hyperlink r:id="rId142" ref="E67"/>
-    <hyperlink r:id="rId143" ref="C68"/>
-    <hyperlink r:id="rId144" ref="D68"/>
-    <hyperlink r:id="rId145" ref="E68"/>
-    <hyperlink r:id="rId146" ref="D69"/>
-    <hyperlink r:id="rId147" ref="E69"/>
-    <hyperlink r:id="rId148" ref="D70"/>
-    <hyperlink r:id="rId149" ref="E70"/>
-    <hyperlink r:id="rId150" ref="C71"/>
-    <hyperlink r:id="rId151" ref="D71"/>
-    <hyperlink r:id="rId152" ref="C72"/>
-    <hyperlink r:id="rId153" ref="D72"/>
-    <hyperlink r:id="rId154" ref="E72"/>
-    <hyperlink r:id="rId155" ref="C73"/>
-    <hyperlink r:id="rId156" ref="D73"/>
-    <hyperlink r:id="rId157" ref="E73"/>
-    <hyperlink r:id="rId158" ref="D76"/>
-    <hyperlink r:id="rId159" ref="E76"/>
-    <hyperlink r:id="rId160" ref="D77"/>
-    <hyperlink r:id="rId161" ref="E77"/>
-    <hyperlink r:id="rId162" ref="D78"/>
-    <hyperlink r:id="rId163" ref="E78"/>
-    <hyperlink r:id="rId164" ref="F78"/>
-    <hyperlink r:id="rId165" ref="D79"/>
-    <hyperlink r:id="rId166" ref="E79"/>
-    <hyperlink r:id="rId167" ref="D80"/>
-    <hyperlink r:id="rId168" ref="E80"/>
-    <hyperlink r:id="rId169" ref="D81"/>
-    <hyperlink r:id="rId170" ref="E81"/>
-    <hyperlink r:id="rId171" ref="D82"/>
-    <hyperlink r:id="rId172" ref="E82"/>
-    <hyperlink r:id="rId173" ref="D83"/>
-    <hyperlink r:id="rId174" ref="E83"/>
-    <hyperlink r:id="rId175" location="callForPapersHeader" ref="D84"/>
-    <hyperlink r:id="rId176" ref="E84"/>
-    <hyperlink r:id="rId177" ref="D85"/>
-    <hyperlink r:id="rId178" ref="F85"/>
-    <hyperlink r:id="rId179" ref="D86"/>
-    <hyperlink r:id="rId180" ref="E86"/>
-    <hyperlink r:id="rId181" ref="F86"/>
-    <hyperlink r:id="rId182" ref="D87"/>
-    <hyperlink r:id="rId183" ref="E87"/>
-    <hyperlink r:id="rId184" ref="D88"/>
-    <hyperlink r:id="rId185" ref="E88"/>
-    <hyperlink r:id="rId186" ref="C89"/>
-    <hyperlink r:id="rId187" ref="D89"/>
-    <hyperlink r:id="rId188" ref="E89"/>
-    <hyperlink r:id="rId189" ref="F89"/>
-    <hyperlink r:id="rId190" ref="C90"/>
-    <hyperlink r:id="rId191" ref="D90"/>
-    <hyperlink r:id="rId192" ref="E90"/>
-    <hyperlink r:id="rId193" ref="F90"/>
-    <hyperlink r:id="rId194" ref="D91"/>
-    <hyperlink r:id="rId195" ref="E91"/>
-    <hyperlink r:id="rId196" ref="D94"/>
-    <hyperlink r:id="rId197" ref="E94"/>
-    <hyperlink r:id="rId198" ref="D96"/>
-    <hyperlink r:id="rId199" ref="D97"/>
-    <hyperlink r:id="rId200" ref="E97"/>
-    <hyperlink r:id="rId201" ref="D98"/>
-    <hyperlink r:id="rId202" ref="D99"/>
-    <hyperlink r:id="rId203" ref="E99"/>
-    <hyperlink r:id="rId204" ref="F99"/>
-    <hyperlink r:id="rId205" ref="C100"/>
-    <hyperlink r:id="rId206" ref="D100"/>
-    <hyperlink r:id="rId207" ref="E100"/>
-    <hyperlink r:id="rId208" ref="D101"/>
-    <hyperlink r:id="rId209" ref="E101"/>
-    <hyperlink r:id="rId210" ref="F101"/>
-    <hyperlink r:id="rId211" ref="D103"/>
-    <hyperlink r:id="rId212" ref="D104"/>
-    <hyperlink r:id="rId213" ref="E104"/>
-    <hyperlink r:id="rId214" ref="D105"/>
-    <hyperlink r:id="rId215" ref="D106"/>
-    <hyperlink r:id="rId216" ref="D107"/>
-    <hyperlink r:id="rId217" ref="E107"/>
-    <hyperlink r:id="rId218" ref="D108"/>
-    <hyperlink r:id="rId219" ref="E108"/>
-    <hyperlink r:id="rId220" ref="D109"/>
-    <hyperlink r:id="rId221" ref="E109"/>
-    <hyperlink r:id="rId222" ref="D110"/>
-    <hyperlink r:id="rId223" ref="E110"/>
-    <hyperlink r:id="rId224" ref="D111"/>
-    <hyperlink r:id="rId225" ref="E111"/>
-    <hyperlink r:id="rId226" ref="D112"/>
-    <hyperlink r:id="rId227" ref="E112"/>
-    <hyperlink r:id="rId228" ref="D113"/>
-    <hyperlink r:id="rId229" ref="E113"/>
-    <hyperlink r:id="rId230" ref="D114"/>
-    <hyperlink r:id="rId231" ref="E114"/>
-    <hyperlink r:id="rId232" ref="F114"/>
-    <hyperlink r:id="rId233" ref="D115"/>
-    <hyperlink r:id="rId234" ref="E115"/>
-    <hyperlink r:id="rId235" ref="D116"/>
-    <hyperlink r:id="rId236" ref="E116"/>
-    <hyperlink r:id="rId237" ref="F116"/>
-    <hyperlink r:id="rId238" ref="D117"/>
-    <hyperlink r:id="rId239" ref="E117"/>
-    <hyperlink r:id="rId240" ref="D118"/>
-    <hyperlink r:id="rId241" ref="E118"/>
-    <hyperlink r:id="rId242" ref="D119"/>
-    <hyperlink r:id="rId243" ref="E119"/>
-    <hyperlink r:id="rId244" ref="D120"/>
-    <hyperlink r:id="rId245" ref="E120"/>
+    <hyperlink r:id="rId114" ref="C56"/>
+    <hyperlink r:id="rId115" ref="D56"/>
+    <hyperlink r:id="rId116" ref="D57"/>
+    <hyperlink r:id="rId117" ref="E57"/>
+    <hyperlink r:id="rId118" location="1069-2509" ref="C58"/>
+    <hyperlink r:id="rId119" location="open-access" ref="D58"/>
+    <hyperlink r:id="rId120" location="1069-2509" ref="F58"/>
+    <hyperlink r:id="rId121" ref="C59"/>
+    <hyperlink r:id="rId122" ref="D59"/>
+    <hyperlink r:id="rId123" ref="E59"/>
+    <hyperlink r:id="rId124" ref="D60"/>
+    <hyperlink r:id="rId125" ref="E60"/>
+    <hyperlink r:id="rId126" ref="D61"/>
+    <hyperlink r:id="rId127" ref="E61"/>
+    <hyperlink r:id="rId128" ref="C62"/>
+    <hyperlink r:id="rId129" ref="D62"/>
+    <hyperlink r:id="rId130" location="Fees%20and%20funding" ref="C63"/>
+    <hyperlink r:id="rId131" ref="D63"/>
+    <hyperlink r:id="rId132" ref="E63"/>
+    <hyperlink r:id="rId133" ref="C64"/>
+    <hyperlink r:id="rId134" ref="D64"/>
+    <hyperlink r:id="rId135" ref="E64"/>
+    <hyperlink r:id="rId136" ref="F64"/>
+    <hyperlink r:id="rId137" ref="C65"/>
+    <hyperlink r:id="rId138" ref="D65"/>
+    <hyperlink r:id="rId139" ref="D66"/>
+    <hyperlink r:id="rId140" ref="E66"/>
+    <hyperlink r:id="rId141" ref="C67"/>
+    <hyperlink r:id="rId142" ref="D67"/>
+    <hyperlink r:id="rId143" ref="E67"/>
+    <hyperlink r:id="rId144" ref="C68"/>
+    <hyperlink r:id="rId145" ref="D68"/>
+    <hyperlink r:id="rId146" ref="E68"/>
+    <hyperlink r:id="rId147" ref="D69"/>
+    <hyperlink r:id="rId148" ref="E69"/>
+    <hyperlink r:id="rId149" ref="D70"/>
+    <hyperlink r:id="rId150" ref="E70"/>
+    <hyperlink r:id="rId151" ref="C71"/>
+    <hyperlink r:id="rId152" ref="D71"/>
+    <hyperlink r:id="rId153" ref="C72"/>
+    <hyperlink r:id="rId154" ref="D72"/>
+    <hyperlink r:id="rId155" ref="E72"/>
+    <hyperlink r:id="rId156" ref="C73"/>
+    <hyperlink r:id="rId157" ref="D73"/>
+    <hyperlink r:id="rId158" ref="E73"/>
+    <hyperlink r:id="rId159" ref="D76"/>
+    <hyperlink r:id="rId160" ref="E76"/>
+    <hyperlink r:id="rId161" ref="D77"/>
+    <hyperlink r:id="rId162" ref="E77"/>
+    <hyperlink r:id="rId163" ref="D78"/>
+    <hyperlink r:id="rId164" ref="E78"/>
+    <hyperlink r:id="rId165" ref="F78"/>
+    <hyperlink r:id="rId166" ref="D79"/>
+    <hyperlink r:id="rId167" ref="E79"/>
+    <hyperlink r:id="rId168" ref="D80"/>
+    <hyperlink r:id="rId169" ref="E80"/>
+    <hyperlink r:id="rId170" ref="D81"/>
+    <hyperlink r:id="rId171" ref="E81"/>
+    <hyperlink r:id="rId172" ref="D82"/>
+    <hyperlink r:id="rId173" ref="E82"/>
+    <hyperlink r:id="rId174" ref="D83"/>
+    <hyperlink r:id="rId175" ref="E83"/>
+    <hyperlink r:id="rId176" location="callForPapersHeader" ref="D84"/>
+    <hyperlink r:id="rId177" ref="E84"/>
+    <hyperlink r:id="rId178" ref="D85"/>
+    <hyperlink r:id="rId179" ref="F85"/>
+    <hyperlink r:id="rId180" ref="D86"/>
+    <hyperlink r:id="rId181" ref="E86"/>
+    <hyperlink r:id="rId182" ref="F86"/>
+    <hyperlink r:id="rId183" ref="D87"/>
+    <hyperlink r:id="rId184" ref="E87"/>
+    <hyperlink r:id="rId185" ref="D88"/>
+    <hyperlink r:id="rId186" ref="E88"/>
+    <hyperlink r:id="rId187" ref="C89"/>
+    <hyperlink r:id="rId188" ref="D89"/>
+    <hyperlink r:id="rId189" ref="E89"/>
+    <hyperlink r:id="rId190" ref="F89"/>
+    <hyperlink r:id="rId191" ref="C90"/>
+    <hyperlink r:id="rId192" ref="D90"/>
+    <hyperlink r:id="rId193" ref="E90"/>
+    <hyperlink r:id="rId194" ref="F90"/>
+    <hyperlink r:id="rId195" ref="D91"/>
+    <hyperlink r:id="rId196" ref="E91"/>
+    <hyperlink r:id="rId197" ref="D94"/>
+    <hyperlink r:id="rId198" ref="E94"/>
+    <hyperlink r:id="rId199" ref="D96"/>
+    <hyperlink r:id="rId200" ref="D97"/>
+    <hyperlink r:id="rId201" ref="E97"/>
+    <hyperlink r:id="rId202" ref="D98"/>
+    <hyperlink r:id="rId203" ref="D99"/>
+    <hyperlink r:id="rId204" ref="E99"/>
+    <hyperlink r:id="rId205" ref="F99"/>
+    <hyperlink r:id="rId206" ref="C100"/>
+    <hyperlink r:id="rId207" ref="D100"/>
+    <hyperlink r:id="rId208" ref="E100"/>
+    <hyperlink r:id="rId209" ref="D101"/>
+    <hyperlink r:id="rId210" ref="E101"/>
+    <hyperlink r:id="rId211" ref="F101"/>
+    <hyperlink r:id="rId212" ref="D103"/>
+    <hyperlink r:id="rId213" ref="D104"/>
+    <hyperlink r:id="rId214" ref="E104"/>
+    <hyperlink r:id="rId215" ref="D105"/>
+    <hyperlink r:id="rId216" ref="D106"/>
+    <hyperlink r:id="rId217" ref="D107"/>
+    <hyperlink r:id="rId218" ref="E107"/>
+    <hyperlink r:id="rId219" ref="D108"/>
+    <hyperlink r:id="rId220" ref="E108"/>
+    <hyperlink r:id="rId221" ref="D109"/>
+    <hyperlink r:id="rId222" ref="E109"/>
+    <hyperlink r:id="rId223" ref="D110"/>
+    <hyperlink r:id="rId224" ref="E110"/>
+    <hyperlink r:id="rId225" ref="D111"/>
+    <hyperlink r:id="rId226" ref="E111"/>
+    <hyperlink r:id="rId227" ref="D112"/>
+    <hyperlink r:id="rId228" ref="E112"/>
+    <hyperlink r:id="rId229" ref="D113"/>
+    <hyperlink r:id="rId230" ref="E113"/>
+    <hyperlink r:id="rId231" ref="D114"/>
+    <hyperlink r:id="rId232" ref="E114"/>
+    <hyperlink r:id="rId233" ref="F114"/>
+    <hyperlink r:id="rId234" ref="D115"/>
+    <hyperlink r:id="rId235" ref="E115"/>
+    <hyperlink r:id="rId236" ref="D116"/>
+    <hyperlink r:id="rId237" ref="E116"/>
+    <hyperlink r:id="rId238" ref="F116"/>
+    <hyperlink r:id="rId239" ref="D117"/>
+    <hyperlink r:id="rId240" ref="E117"/>
+    <hyperlink r:id="rId241" ref="D118"/>
+    <hyperlink r:id="rId242" ref="E118"/>
+    <hyperlink r:id="rId243" ref="D119"/>
+    <hyperlink r:id="rId244" ref="E119"/>
+    <hyperlink r:id="rId245" ref="D120"/>
+    <hyperlink r:id="rId246" ref="E120"/>
   </hyperlinks>
-  <drawing r:id="rId246"/>
+  <drawing r:id="rId247"/>
 </worksheet>
 </file>
 
@@ -14494,12 +14507,24 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="83"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="81"/>
+      <c r="A7" s="74" t="s">
+        <v>485</v>
+      </c>
+      <c r="B7" s="75">
+        <v>3.0</v>
+      </c>
+      <c r="C7" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>486</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>487</v>
+      </c>
+      <c r="F7" s="76" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="83"/>
@@ -22457,8 +22482,12 @@
     <hyperlink r:id="rId8" ref="D5"/>
     <hyperlink r:id="rId9" ref="D6"/>
     <hyperlink r:id="rId10" ref="E6"/>
+    <hyperlink r:id="rId11" ref="C7"/>
+    <hyperlink r:id="rId12" ref="D7"/>
+    <hyperlink r:id="rId13" ref="E7"/>
+    <hyperlink r:id="rId14" ref="F7"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -22477,22 +22506,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="85" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="C1" s="71" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="E1" s="72" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="70" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G1" s="73"/>
       <c r="H1" s="73"/>
@@ -22517,22 +22546,22 @@
     </row>
     <row r="2">
       <c r="A2" s="86" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B2" s="86" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="C2" s="86" t="s">
         <v>55</v>
       </c>
       <c r="D2" s="86" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="E2" s="87" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="F2" s="86" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="G2" s="88"/>
       <c r="H2" s="88"/>
@@ -22725,7 +22754,7 @@
     </row>
     <row r="9">
       <c r="A9" s="86" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B9" s="88"/>
       <c r="C9" s="88"/>
@@ -22755,7 +22784,7 @@
     </row>
     <row r="10">
       <c r="A10" s="90" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="B10" s="88"/>
       <c r="C10" s="88"/>
@@ -26303,39 +26332,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="85" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="C1" s="71" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="E1" s="72" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="70" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="92" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="C2" s="92" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="D2" s="93">
         <v>45746.0</v>
       </c>
       <c r="E2" s="94" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="F2" s="95" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -26360,42 +26389,42 @@
     <row r="1">
       <c r="A1" s="96"/>
       <c r="B1" s="97" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="C1" s="96"/>
     </row>
     <row r="2">
       <c r="A2" s="96"/>
       <c r="B2" s="98" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="C2" s="96"/>
     </row>
     <row r="3">
       <c r="A3" s="96"/>
       <c r="B3" s="98" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="C3" s="96"/>
     </row>
     <row r="4">
       <c r="A4" s="96"/>
       <c r="B4" s="98" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="C4" s="96"/>
     </row>
     <row r="5">
       <c r="A5" s="96"/>
       <c r="B5" s="98" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="C5" s="96"/>
     </row>
     <row r="6">
       <c r="A6" s="99"/>
       <c r="B6" s="98" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="C6" s="96"/>
     </row>
@@ -26428,82 +26457,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="100" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="B1" s="100" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="101" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="B2" s="101" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="101" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="B3" s="101" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="101" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="B4" s="101" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="101" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="B5" s="101" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="101" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="B6" s="101" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="101" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="B7" s="101" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="101" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="B8" s="101" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="101" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="B9" s="101" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="101" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="B10" s="101" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Added plos one journal
</commit_message>
<xml_diff>
--- a/source/Journals.xlsx
+++ b/source/Journals.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="570">
   <si>
     <t>Journal</t>
   </si>
@@ -1190,6 +1190,34 @@
   </si>
   <si>
     <t>time to publish &lt;= 90 days</t>
+  </si>
+  <si>
+    <t>PLoS ONE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>1000 USD</t>
+    </r>
+  </si>
+  <si>
+    <t>https://journals.plos.org/plosone/</t>
+  </si>
+  <si>
+    <t>https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0329589</t>
+  </si>
+  <si>
+    <t>time to publish ~ 200 days</t>
   </si>
   <si>
     <t>Decision Sciences</t>
@@ -4561,115 +4589,115 @@
       <c r="G75" s="12"/>
     </row>
     <row r="76">
-      <c r="A76" s="7"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="27"/>
+      <c r="A76" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="F76" s="25" t="s">
+        <v>318</v>
+      </c>
       <c r="G76" s="12"/>
     </row>
     <row r="77">
-      <c r="A77" s="43" t="s">
-        <v>314</v>
-      </c>
-      <c r="B77" s="44"/>
-      <c r="C77" s="45"/>
-      <c r="D77" s="46"/>
-      <c r="E77" s="47"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="48"/>
+      <c r="A77" s="7"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="12"/>
     </row>
     <row r="78">
-      <c r="A78" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="B78" s="8" t="s">
+      <c r="A78" s="43" t="s">
+        <v>319</v>
+      </c>
+      <c r="B78" s="44"/>
+      <c r="C78" s="45"/>
+      <c r="D78" s="46"/>
+      <c r="E78" s="47"/>
+      <c r="F78" s="45"/>
+      <c r="G78" s="48"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B79" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C78" s="25" t="s">
+      <c r="C79" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D78" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="F78" s="27" t="s">
-        <v>318</v>
-      </c>
-      <c r="G78" s="12"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="7"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="27"/>
+      <c r="D79" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="F79" s="27" t="s">
+        <v>323</v>
+      </c>
       <c r="G79" s="12"/>
     </row>
     <row r="80">
-      <c r="A80" s="43" t="s">
-        <v>319</v>
-      </c>
-      <c r="B80" s="44"/>
-      <c r="C80" s="45"/>
-      <c r="D80" s="46"/>
-      <c r="E80" s="47"/>
-      <c r="F80" s="45"/>
-      <c r="G80" s="48"/>
+      <c r="A80" s="7"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="27"/>
+      <c r="G80" s="12"/>
     </row>
     <row r="81">
-      <c r="A81" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="B81" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="D81" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="E81" s="15" t="s">
-        <v>323</v>
-      </c>
-      <c r="F81" s="9"/>
-      <c r="G81" s="12"/>
+      <c r="A81" s="43" t="s">
+        <v>324</v>
+      </c>
+      <c r="B81" s="44"/>
+      <c r="C81" s="45"/>
+      <c r="D81" s="46"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="45"/>
+      <c r="G81" s="48"/>
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B82" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C82" s="49" t="s">
-        <v>9</v>
+      <c r="C82" s="9" t="s">
+        <v>326</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="F82" s="11" t="s">
-        <v>327</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="F82" s="9"/>
       <c r="G82" s="12"/>
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B83" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C83" s="9" t="s">
-        <v>329</v>
+      <c r="C83" s="49" t="s">
+        <v>9</v>
       </c>
       <c r="D83" s="15" t="s">
         <v>330</v>
@@ -4677,7 +4705,7 @@
       <c r="E83" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="F83" s="25" t="s">
+      <c r="F83" s="11" t="s">
         <v>332</v>
       </c>
       <c r="G83" s="12"/>
@@ -4690,33 +4718,33 @@
         <v>8</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>50</v>
+        <v>334</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="F84" s="11" t="s">
         <v>336</v>
+      </c>
+      <c r="F84" s="25" t="s">
+        <v>337</v>
       </c>
       <c r="G84" s="12"/>
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="B85" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B85" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C85" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="D85" s="16" t="s">
+      <c r="C85" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D85" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="E85" s="24" t="s">
+      <c r="E85" s="15" t="s">
         <v>340</v>
       </c>
       <c r="F85" s="11" t="s">
@@ -4728,40 +4756,40 @@
       <c r="A86" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C86" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" s="15" t="s">
+      <c r="C86" s="11" t="s">
         <v>343</v>
       </c>
-      <c r="E86" s="15" t="s">
+      <c r="D86" s="16" t="s">
         <v>344</v>
       </c>
+      <c r="E86" s="24" t="s">
+        <v>345</v>
+      </c>
       <c r="F86" s="11" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="G86" s="12"/>
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C87" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="D87" s="10" t="s">
+      <c r="B87" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D87" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="E87" s="10" t="s">
+      <c r="E87" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="F87" s="50" t="s">
+      <c r="F87" s="11" t="s">
         <v>350</v>
       </c>
       <c r="G87" s="12"/>
@@ -4770,67 +4798,67 @@
       <c r="A88" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="F88" s="50" t="s">
+        <v>355</v>
+      </c>
+      <c r="G88" s="12"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B89" s="14" t="s">
         <v>8</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D88" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="E88" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="F88" s="11" t="s">
-        <v>354</v>
-      </c>
-      <c r="G88" s="12"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="51" t="s">
-        <v>355</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="C89" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D89" s="15" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E89" s="15" t="s">
-        <v>357</v>
-      </c>
-      <c r="F89" s="9" t="s">
         <v>358</v>
       </c>
+      <c r="F89" s="11" t="s">
+        <v>359</v>
+      </c>
       <c r="G89" s="12"/>
     </row>
     <row r="90">
-      <c r="A90" s="52" t="s">
-        <v>359</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C90" s="11" t="s">
+      <c r="A90" s="51" t="s">
         <v>360</v>
       </c>
-      <c r="D90" s="10" t="s">
+      <c r="B90" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="E90" s="30" t="s">
+      <c r="E90" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="F90" s="25" t="s">
+      <c r="F90" s="9" t="s">
         <v>363</v>
       </c>
       <c r="G90" s="12"/>
     </row>
     <row r="91">
-      <c r="A91" s="53" t="s">
+      <c r="A91" s="52" t="s">
         <v>364</v>
       </c>
       <c r="B91" s="8" t="s">
@@ -4839,10 +4867,10 @@
       <c r="C91" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="D91" s="16" t="s">
+      <c r="D91" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="E91" s="30" t="s">
         <v>367</v>
       </c>
       <c r="F91" s="25" t="s">
@@ -4851,22 +4879,22 @@
       <c r="G91" s="12"/>
     </row>
     <row r="92">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="53" t="s">
         <v>369</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C92" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="D92" s="10" t="s">
+      <c r="D92" s="16" t="s">
         <v>371</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>372</v>
       </c>
-      <c r="F92" s="27" t="s">
+      <c r="F92" s="25" t="s">
         <v>373</v>
       </c>
       <c r="G92" s="12"/>
@@ -4876,52 +4904,52 @@
         <v>374</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>375</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F93" s="27" t="s">
-        <v>277</v>
+        <v>378</v>
       </c>
       <c r="G93" s="12"/>
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="25" t="s">
-        <v>182</v>
+      <c r="C94" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="F94" s="25" t="s">
-        <v>380</v>
+        <v>381</v>
+      </c>
+      <c r="F94" s="27" t="s">
+        <v>277</v>
       </c>
       <c r="G94" s="12"/>
     </row>
     <row r="95">
-      <c r="A95" s="28" t="s">
-        <v>381</v>
+      <c r="A95" s="7" t="s">
+        <v>382</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C95" s="25" t="s">
-        <v>382</v>
+        <v>182</v>
       </c>
       <c r="D95" s="10" t="s">
         <v>383</v>
@@ -4935,180 +4963,180 @@
       <c r="G95" s="12"/>
     </row>
     <row r="96">
-      <c r="A96" s="54" t="s">
+      <c r="A96" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="25" t="s">
+        <v>387</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="F96" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="G96" s="12"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B96" s="55" t="s">
+      <c r="B97" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="C97" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D96" s="56" t="s">
+      <c r="D97" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="E96" s="57" t="s">
-        <v>386</v>
-      </c>
-      <c r="F96" s="54" t="s">
+      <c r="E97" s="57" t="s">
+        <v>391</v>
+      </c>
+      <c r="F97" s="54" t="s">
         <v>235</v>
       </c>
-      <c r="G96" s="58"/>
-    </row>
-    <row r="97">
-      <c r="A97" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="B97" s="8" t="s">
+      <c r="G97" s="58"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B98" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C97" s="25" t="s">
+      <c r="C98" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D97" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="F97" s="27" t="s">
-        <v>390</v>
-      </c>
-      <c r="G97" s="12"/>
-    </row>
-    <row r="98">
-      <c r="A98" s="59"/>
-      <c r="B98" s="60"/>
-      <c r="C98" s="59"/>
-      <c r="D98" s="60"/>
-      <c r="E98" s="61"/>
-      <c r="F98" s="59"/>
-      <c r="G98" s="41"/>
+      <c r="D98" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="F98" s="27" t="s">
+        <v>395</v>
+      </c>
+      <c r="G98" s="12"/>
     </row>
     <row r="99">
-      <c r="A99" s="43" t="s">
-        <v>391</v>
-      </c>
-      <c r="B99" s="44"/>
-      <c r="C99" s="45"/>
-      <c r="D99" s="46"/>
-      <c r="E99" s="47"/>
-      <c r="F99" s="45"/>
-      <c r="G99" s="48"/>
+      <c r="A99" s="59"/>
+      <c r="B99" s="60"/>
+      <c r="C99" s="59"/>
+      <c r="D99" s="60"/>
+      <c r="E99" s="61"/>
+      <c r="F99" s="59"/>
+      <c r="G99" s="41"/>
     </row>
     <row r="100">
-      <c r="A100" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="B100" s="8" t="s">
+      <c r="A100" s="43" t="s">
+        <v>396</v>
+      </c>
+      <c r="B100" s="44"/>
+      <c r="C100" s="45"/>
+      <c r="D100" s="46"/>
+      <c r="E100" s="47"/>
+      <c r="F100" s="45"/>
+      <c r="G100" s="48"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="B101" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C100" s="11" t="s">
+      <c r="C101" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D100" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="E100" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="F100" s="27"/>
-      <c r="G100" s="12"/>
-    </row>
-    <row r="101">
-      <c r="A101" s="7"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="30"/>
-      <c r="E101" s="30"/>
+      <c r="D101" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>399</v>
+      </c>
       <c r="F101" s="27"/>
       <c r="G101" s="12"/>
     </row>
     <row r="102">
-      <c r="A102" s="43" t="s">
-        <v>395</v>
-      </c>
-      <c r="B102" s="44"/>
-      <c r="C102" s="45"/>
-      <c r="D102" s="46" t="s">
-        <v>396</v>
-      </c>
-      <c r="E102" s="47"/>
-      <c r="F102" s="45"/>
-      <c r="G102" s="48"/>
+      <c r="A102" s="7"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="30"/>
+      <c r="E102" s="30"/>
+      <c r="F102" s="27"/>
+      <c r="G102" s="12"/>
     </row>
     <row r="103">
-      <c r="A103" s="28" t="s">
-        <v>397</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C103" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="D103" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="E103" s="26" t="s">
-        <v>399</v>
-      </c>
-      <c r="F103" s="11" t="s">
+      <c r="A103" s="43" t="s">
         <v>400</v>
       </c>
-      <c r="G103" s="12"/>
+      <c r="B103" s="44"/>
+      <c r="C103" s="45"/>
+      <c r="D103" s="46" t="s">
+        <v>401</v>
+      </c>
+      <c r="E103" s="47"/>
+      <c r="F103" s="45"/>
+      <c r="G103" s="48"/>
     </row>
     <row r="104">
-      <c r="A104" s="7" t="s">
-        <v>401</v>
+      <c r="A104" s="28" t="s">
+        <v>402</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>402</v>
+        <v>293</v>
       </c>
       <c r="D104" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="E104" s="62" t="s">
-        <v>55</v>
+      <c r="E104" s="26" t="s">
+        <v>404</v>
       </c>
       <c r="F104" s="11" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="G104" s="12"/>
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C105" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="D105" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="E105" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="F105" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="G105" s="12"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="D105" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="E105" s="10" t="s">
-        <v>407</v>
-      </c>
-      <c r="F105" s="25" t="s">
-        <v>408</v>
-      </c>
-      <c r="G105" s="12"/>
-    </row>
-    <row r="106">
-      <c r="A106" s="28" t="s">
-        <v>409</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C106" s="25" t="s">
-        <v>410</v>
       </c>
       <c r="D106" s="10" t="s">
         <v>411</v>
@@ -5116,92 +5144,92 @@
       <c r="E106" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="F106" s="27" t="s">
+      <c r="F106" s="25" t="s">
         <v>413</v>
       </c>
       <c r="G106" s="12"/>
     </row>
     <row r="107">
-      <c r="A107" s="7" t="s">
+      <c r="A107" s="28" t="s">
         <v>414</v>
       </c>
       <c r="B107" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="C107" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="E107" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="F107" s="27" t="s">
+        <v>418</v>
+      </c>
+      <c r="G107" s="12"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C108" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D107" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="E107" s="63" t="s">
-        <v>416</v>
-      </c>
-      <c r="F107" s="25" t="s">
-        <v>417</v>
-      </c>
-      <c r="G107" s="12"/>
-    </row>
-    <row r="108">
-      <c r="A108" s="13"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="9"/>
-      <c r="D108" s="64"/>
-      <c r="E108" s="64"/>
-      <c r="F108" s="9"/>
+      <c r="D108" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="E108" s="63" t="s">
+        <v>421</v>
+      </c>
+      <c r="F108" s="25" t="s">
+        <v>422</v>
+      </c>
       <c r="G108" s="12"/>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="B109" s="44"/>
-      <c r="C109" s="45"/>
-      <c r="D109" s="65" t="s">
-        <v>419</v>
-      </c>
-      <c r="E109" s="47"/>
-      <c r="F109" s="45"/>
-      <c r="G109" s="48"/>
+      <c r="A109" s="13"/>
+      <c r="B109" s="14"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="64"/>
+      <c r="E109" s="64"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="12"/>
     </row>
     <row r="110">
-      <c r="A110" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="B110" s="8" t="s">
+      <c r="A110" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B110" s="44"/>
+      <c r="C110" s="45"/>
+      <c r="D110" s="65" t="s">
+        <v>424</v>
+      </c>
+      <c r="E110" s="47"/>
+      <c r="F110" s="45"/>
+      <c r="G110" s="48"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C110" s="9" t="s">
+      <c r="C111" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D110" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="E110" s="26" t="s">
-        <v>422</v>
-      </c>
-      <c r="F110" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="G110" s="12"/>
-    </row>
-    <row r="111">
-      <c r="A111" s="13" t="s">
-        <v>424</v>
-      </c>
-      <c r="B111" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="D111" s="15" t="s">
+      <c r="D111" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="E111" s="64" t="s">
+      <c r="E111" s="26" t="s">
         <v>427</v>
       </c>
-      <c r="F111" s="9" t="s">
+      <c r="F111" s="11" t="s">
         <v>428</v>
       </c>
       <c r="G111" s="12"/>
@@ -5210,8 +5238,8 @@
       <c r="A112" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="B112" s="8" t="s">
-        <v>30</v>
+      <c r="B112" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="C112" s="9" t="s">
         <v>430</v>
@@ -5220,174 +5248,174 @@
         <v>431</v>
       </c>
       <c r="E112" s="64" t="s">
-        <v>427</v>
-      </c>
-      <c r="F112" s="9"/>
+        <v>432</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>433</v>
+      </c>
       <c r="G112" s="12"/>
     </row>
     <row r="113">
       <c r="A113" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>436</v>
+      </c>
+      <c r="E113" s="64" t="s">
         <v>432</v>
-      </c>
-      <c r="B113" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="D113" s="15" t="s">
-        <v>434</v>
-      </c>
-      <c r="E113" s="15" t="s">
-        <v>435</v>
       </c>
       <c r="F113" s="9"/>
       <c r="G113" s="12"/>
     </row>
     <row r="114">
       <c r="A114" s="13" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B114" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D114" s="15" t="s">
-        <v>438</v>
-      </c>
-      <c r="E114" s="66" t="s">
         <v>439</v>
+      </c>
+      <c r="E114" s="15" t="s">
+        <v>440</v>
       </c>
       <c r="F114" s="9"/>
       <c r="G114" s="12"/>
     </row>
     <row r="115">
       <c r="A115" s="13" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="D115" s="15" t="s">
-        <v>441</v>
-      </c>
-      <c r="E115" s="15" t="s">
-        <v>442</v>
+        <v>443</v>
+      </c>
+      <c r="E115" s="66" t="s">
+        <v>444</v>
       </c>
       <c r="F115" s="9"/>
       <c r="G115" s="12"/>
     </row>
     <row r="116">
       <c r="A116" s="13" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="D116" s="15" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="E116" s="15" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="F116" s="9"/>
       <c r="G116" s="12"/>
     </row>
     <row r="117">
-      <c r="A117" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="B117" s="8" t="s">
+      <c r="A117" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="B117" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="D117" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="E117" s="10" t="s">
-        <v>448</v>
+        <v>442</v>
+      </c>
+      <c r="D117" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="E117" s="15" t="s">
+        <v>450</v>
       </c>
       <c r="F117" s="9"/>
       <c r="G117" s="12"/>
     </row>
     <row r="118">
       <c r="A118" s="7" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C118" s="11" t="s">
-        <v>450</v>
+      <c r="C118" s="9" t="s">
+        <v>438</v>
       </c>
       <c r="D118" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="E118" s="24" t="s">
         <v>452</v>
+      </c>
+      <c r="E118" s="10" t="s">
+        <v>453</v>
       </c>
       <c r="F118" s="9"/>
       <c r="G118" s="12"/>
     </row>
     <row r="119">
       <c r="A119" s="7" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B119" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>437</v>
+        <v>455</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="E119" s="10" t="s">
-        <v>455</v>
+        <v>456</v>
+      </c>
+      <c r="E119" s="24" t="s">
+        <v>457</v>
       </c>
       <c r="F119" s="9"/>
       <c r="G119" s="12"/>
     </row>
     <row r="120">
       <c r="A120" s="7" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B120" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="E120" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="F120" s="25" t="s">
-        <v>459</v>
-      </c>
+        <v>460</v>
+      </c>
+      <c r="F120" s="9"/>
       <c r="G120" s="12"/>
     </row>
     <row r="121">
       <c r="A121" s="7" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B121" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
       <c r="D121" s="10" t="s">
         <v>462</v>
@@ -5395,28 +5423,28 @@
       <c r="E121" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="F121" s="27"/>
+      <c r="F121" s="25" t="s">
+        <v>464</v>
+      </c>
       <c r="G121" s="12"/>
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E122" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="F122" s="25" t="s">
         <v>468</v>
       </c>
+      <c r="F122" s="27"/>
       <c r="G122" s="12"/>
     </row>
     <row r="123">
@@ -5424,87 +5452,99 @@
         <v>469</v>
       </c>
       <c r="B123" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="D123" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="E123" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="F123" s="25" t="s">
+        <v>473</v>
+      </c>
+      <c r="G123" s="12"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="B124" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C123" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="D123" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="E123" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="F123" s="27"/>
-      <c r="G123" s="12"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="13" t="s">
-        <v>472</v>
-      </c>
-      <c r="B124" s="14" t="s">
+      <c r="C124" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="D124" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>476</v>
+      </c>
+      <c r="F124" s="27"/>
+      <c r="G124" s="12"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="B125" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C124" s="9" t="s">
+      <c r="C125" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D124" s="15" t="s">
-        <v>473</v>
-      </c>
-      <c r="E124" s="15" t="s">
+      <c r="D125" s="15" t="s">
+        <v>478</v>
+      </c>
+      <c r="E125" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F124" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="G124" s="12"/>
-    </row>
-    <row r="125">
-      <c r="A125" s="53" t="s">
-        <v>475</v>
-      </c>
-      <c r="B125" s="8" t="s">
+      <c r="F125" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="G125" s="12"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="53" t="s">
+        <v>480</v>
+      </c>
+      <c r="B126" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C125" s="11" t="s">
+      <c r="C126" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D125" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="E125" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="F125" s="27" t="s">
-        <v>478</v>
-      </c>
-      <c r="G125" s="12"/>
-    </row>
-    <row r="126">
-      <c r="A126" s="7" t="s">
+      <c r="D126" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="E126" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="F126" s="27" t="s">
+        <v>483</v>
+      </c>
+      <c r="G126" s="12"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="B127" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C126" s="11" t="s">
+      <c r="C127" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D126" s="26" t="s">
-        <v>479</v>
-      </c>
-      <c r="E126" s="10" t="s">
-        <v>480</v>
-      </c>
-      <c r="F126" s="9"/>
-      <c r="G126" s="12"/>
-    </row>
-    <row r="127">
-      <c r="A127" s="13"/>
-      <c r="B127" s="14"/>
-      <c r="C127" s="9"/>
-      <c r="D127" s="64"/>
-      <c r="E127" s="64"/>
+      <c r="D127" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="E127" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="F127" s="9"/>
       <c r="G127" s="12"/>
     </row>
@@ -5520,7 +5560,7 @@
     <row r="129">
       <c r="A129" s="13"/>
       <c r="B129" s="14"/>
-      <c r="C129" s="27"/>
+      <c r="C129" s="9"/>
       <c r="D129" s="64"/>
       <c r="E129" s="64"/>
       <c r="F129" s="9"/>
@@ -5529,7 +5569,7 @@
     <row r="130">
       <c r="A130" s="13"/>
       <c r="B130" s="14"/>
-      <c r="C130" s="11"/>
+      <c r="C130" s="27"/>
       <c r="D130" s="64"/>
       <c r="E130" s="64"/>
       <c r="F130" s="9"/>
@@ -5564,7 +5604,7 @@
     </row>
     <row r="134">
       <c r="A134" s="13"/>
-      <c r="B134" s="67"/>
+      <c r="B134" s="14"/>
       <c r="C134" s="11"/>
       <c r="D134" s="64"/>
       <c r="E134" s="64"/>
@@ -5573,7 +5613,7 @@
     </row>
     <row r="135">
       <c r="A135" s="13"/>
-      <c r="B135" s="14"/>
+      <c r="B135" s="67"/>
       <c r="C135" s="11"/>
       <c r="D135" s="64"/>
       <c r="E135" s="64"/>
@@ -5583,7 +5623,7 @@
     <row r="136">
       <c r="A136" s="13"/>
       <c r="B136" s="14"/>
-      <c r="C136" s="9"/>
+      <c r="C136" s="11"/>
       <c r="D136" s="64"/>
       <c r="E136" s="64"/>
       <c r="F136" s="9"/>
@@ -14309,6 +14349,15 @@
       <c r="E1105" s="64"/>
       <c r="F1105" s="9"/>
       <c r="G1105" s="12"/>
+    </row>
+    <row r="1106">
+      <c r="A1106" s="13"/>
+      <c r="B1106" s="14"/>
+      <c r="C1106" s="9"/>
+      <c r="D1106" s="64"/>
+      <c r="E1106" s="64"/>
+      <c r="F1106" s="9"/>
+      <c r="G1106" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -14477,102 +14526,106 @@
     <hyperlink r:id="rId163" ref="C75"/>
     <hyperlink r:id="rId164" ref="D75"/>
     <hyperlink r:id="rId165" ref="E75"/>
-    <hyperlink r:id="rId166" location="aims-and-scope" ref="C78"/>
-    <hyperlink r:id="rId167" ref="D78"/>
-    <hyperlink r:id="rId168" ref="E78"/>
-    <hyperlink r:id="rId169" ref="D81"/>
-    <hyperlink r:id="rId170" ref="E81"/>
-    <hyperlink r:id="rId171" ref="D82"/>
-    <hyperlink r:id="rId172" ref="E82"/>
-    <hyperlink r:id="rId173" ref="D83"/>
-    <hyperlink r:id="rId174" ref="E83"/>
-    <hyperlink r:id="rId175" ref="F83"/>
-    <hyperlink r:id="rId176" ref="D84"/>
-    <hyperlink r:id="rId177" ref="E84"/>
-    <hyperlink r:id="rId178" ref="D85"/>
-    <hyperlink r:id="rId179" ref="E85"/>
-    <hyperlink r:id="rId180" ref="D86"/>
-    <hyperlink r:id="rId181" ref="E86"/>
-    <hyperlink r:id="rId182" ref="D87"/>
-    <hyperlink r:id="rId183" ref="E87"/>
-    <hyperlink r:id="rId184" ref="D88"/>
-    <hyperlink r:id="rId185" ref="E88"/>
-    <hyperlink r:id="rId186" location="callForPapersHeader" ref="D89"/>
-    <hyperlink r:id="rId187" ref="E89"/>
-    <hyperlink r:id="rId188" ref="D90"/>
-    <hyperlink r:id="rId189" ref="F90"/>
-    <hyperlink r:id="rId190" ref="D91"/>
-    <hyperlink r:id="rId191" ref="E91"/>
-    <hyperlink r:id="rId192" ref="F91"/>
-    <hyperlink r:id="rId193" ref="D92"/>
-    <hyperlink r:id="rId194" ref="E92"/>
-    <hyperlink r:id="rId195" ref="D93"/>
-    <hyperlink r:id="rId196" ref="E93"/>
-    <hyperlink r:id="rId197" ref="C94"/>
-    <hyperlink r:id="rId198" ref="D94"/>
-    <hyperlink r:id="rId199" ref="E94"/>
-    <hyperlink r:id="rId200" ref="F94"/>
+    <hyperlink r:id="rId166" ref="C76"/>
+    <hyperlink r:id="rId167" ref="D76"/>
+    <hyperlink r:id="rId168" ref="E76"/>
+    <hyperlink r:id="rId169" ref="F76"/>
+    <hyperlink r:id="rId170" location="aims-and-scope" ref="C79"/>
+    <hyperlink r:id="rId171" ref="D79"/>
+    <hyperlink r:id="rId172" ref="E79"/>
+    <hyperlink r:id="rId173" ref="D82"/>
+    <hyperlink r:id="rId174" ref="E82"/>
+    <hyperlink r:id="rId175" ref="D83"/>
+    <hyperlink r:id="rId176" ref="E83"/>
+    <hyperlink r:id="rId177" ref="D84"/>
+    <hyperlink r:id="rId178" ref="E84"/>
+    <hyperlink r:id="rId179" ref="F84"/>
+    <hyperlink r:id="rId180" ref="D85"/>
+    <hyperlink r:id="rId181" ref="E85"/>
+    <hyperlink r:id="rId182" ref="D86"/>
+    <hyperlink r:id="rId183" ref="E86"/>
+    <hyperlink r:id="rId184" ref="D87"/>
+    <hyperlink r:id="rId185" ref="E87"/>
+    <hyperlink r:id="rId186" ref="D88"/>
+    <hyperlink r:id="rId187" ref="E88"/>
+    <hyperlink r:id="rId188" ref="D89"/>
+    <hyperlink r:id="rId189" ref="E89"/>
+    <hyperlink r:id="rId190" location="callForPapersHeader" ref="D90"/>
+    <hyperlink r:id="rId191" ref="E90"/>
+    <hyperlink r:id="rId192" ref="D91"/>
+    <hyperlink r:id="rId193" ref="F91"/>
+    <hyperlink r:id="rId194" ref="D92"/>
+    <hyperlink r:id="rId195" ref="E92"/>
+    <hyperlink r:id="rId196" ref="F92"/>
+    <hyperlink r:id="rId197" ref="D93"/>
+    <hyperlink r:id="rId198" ref="E93"/>
+    <hyperlink r:id="rId199" ref="D94"/>
+    <hyperlink r:id="rId200" ref="E94"/>
     <hyperlink r:id="rId201" ref="C95"/>
     <hyperlink r:id="rId202" ref="D95"/>
     <hyperlink r:id="rId203" ref="E95"/>
     <hyperlink r:id="rId204" ref="F95"/>
-    <hyperlink r:id="rId205" ref="D96"/>
-    <hyperlink r:id="rId206" ref="E96"/>
-    <hyperlink r:id="rId207" ref="C97"/>
-    <hyperlink r:id="rId208" ref="D97"/>
-    <hyperlink r:id="rId209" ref="E97"/>
-    <hyperlink r:id="rId210" ref="D100"/>
-    <hyperlink r:id="rId211" ref="E100"/>
-    <hyperlink r:id="rId212" ref="D102"/>
-    <hyperlink r:id="rId213" ref="D103"/>
-    <hyperlink r:id="rId214" ref="E103"/>
-    <hyperlink r:id="rId215" ref="D104"/>
-    <hyperlink r:id="rId216" ref="D105"/>
-    <hyperlink r:id="rId217" ref="E105"/>
-    <hyperlink r:id="rId218" ref="F105"/>
-    <hyperlink r:id="rId219" ref="C106"/>
+    <hyperlink r:id="rId205" ref="C96"/>
+    <hyperlink r:id="rId206" ref="D96"/>
+    <hyperlink r:id="rId207" ref="E96"/>
+    <hyperlink r:id="rId208" ref="F96"/>
+    <hyperlink r:id="rId209" ref="D97"/>
+    <hyperlink r:id="rId210" ref="E97"/>
+    <hyperlink r:id="rId211" ref="C98"/>
+    <hyperlink r:id="rId212" ref="D98"/>
+    <hyperlink r:id="rId213" ref="E98"/>
+    <hyperlink r:id="rId214" ref="D101"/>
+    <hyperlink r:id="rId215" ref="E101"/>
+    <hyperlink r:id="rId216" ref="D103"/>
+    <hyperlink r:id="rId217" ref="D104"/>
+    <hyperlink r:id="rId218" ref="E104"/>
+    <hyperlink r:id="rId219" ref="D105"/>
     <hyperlink r:id="rId220" ref="D106"/>
     <hyperlink r:id="rId221" ref="E106"/>
-    <hyperlink r:id="rId222" ref="D107"/>
-    <hyperlink r:id="rId223" ref="E107"/>
-    <hyperlink r:id="rId224" ref="F107"/>
-    <hyperlink r:id="rId225" ref="D109"/>
-    <hyperlink r:id="rId226" ref="D110"/>
-    <hyperlink r:id="rId227" ref="E110"/>
-    <hyperlink r:id="rId228" ref="D111"/>
-    <hyperlink r:id="rId229" ref="D112"/>
-    <hyperlink r:id="rId230" ref="D113"/>
-    <hyperlink r:id="rId231" ref="E113"/>
-    <hyperlink r:id="rId232" ref="D114"/>
-    <hyperlink r:id="rId233" ref="E114"/>
-    <hyperlink r:id="rId234" ref="D115"/>
-    <hyperlink r:id="rId235" ref="E115"/>
-    <hyperlink r:id="rId236" ref="D116"/>
-    <hyperlink r:id="rId237" ref="E116"/>
-    <hyperlink r:id="rId238" ref="D117"/>
-    <hyperlink r:id="rId239" ref="E117"/>
-    <hyperlink r:id="rId240" ref="D118"/>
-    <hyperlink r:id="rId241" ref="E118"/>
-    <hyperlink r:id="rId242" ref="D119"/>
-    <hyperlink r:id="rId243" ref="E119"/>
-    <hyperlink r:id="rId244" ref="D120"/>
-    <hyperlink r:id="rId245" ref="E120"/>
-    <hyperlink r:id="rId246" ref="F120"/>
-    <hyperlink r:id="rId247" ref="D121"/>
-    <hyperlink r:id="rId248" ref="E121"/>
-    <hyperlink r:id="rId249" ref="D122"/>
-    <hyperlink r:id="rId250" ref="E122"/>
-    <hyperlink r:id="rId251" ref="F122"/>
-    <hyperlink r:id="rId252" ref="D123"/>
-    <hyperlink r:id="rId253" ref="E123"/>
-    <hyperlink r:id="rId254" ref="D124"/>
-    <hyperlink r:id="rId255" ref="E124"/>
-    <hyperlink r:id="rId256" ref="D125"/>
-    <hyperlink r:id="rId257" ref="E125"/>
-    <hyperlink r:id="rId258" ref="D126"/>
-    <hyperlink r:id="rId259" ref="E126"/>
+    <hyperlink r:id="rId222" ref="F106"/>
+    <hyperlink r:id="rId223" ref="C107"/>
+    <hyperlink r:id="rId224" ref="D107"/>
+    <hyperlink r:id="rId225" ref="E107"/>
+    <hyperlink r:id="rId226" ref="D108"/>
+    <hyperlink r:id="rId227" ref="E108"/>
+    <hyperlink r:id="rId228" ref="F108"/>
+    <hyperlink r:id="rId229" ref="D110"/>
+    <hyperlink r:id="rId230" ref="D111"/>
+    <hyperlink r:id="rId231" ref="E111"/>
+    <hyperlink r:id="rId232" ref="D112"/>
+    <hyperlink r:id="rId233" ref="D113"/>
+    <hyperlink r:id="rId234" ref="D114"/>
+    <hyperlink r:id="rId235" ref="E114"/>
+    <hyperlink r:id="rId236" ref="D115"/>
+    <hyperlink r:id="rId237" ref="E115"/>
+    <hyperlink r:id="rId238" ref="D116"/>
+    <hyperlink r:id="rId239" ref="E116"/>
+    <hyperlink r:id="rId240" ref="D117"/>
+    <hyperlink r:id="rId241" ref="E117"/>
+    <hyperlink r:id="rId242" ref="D118"/>
+    <hyperlink r:id="rId243" ref="E118"/>
+    <hyperlink r:id="rId244" ref="D119"/>
+    <hyperlink r:id="rId245" ref="E119"/>
+    <hyperlink r:id="rId246" ref="D120"/>
+    <hyperlink r:id="rId247" ref="E120"/>
+    <hyperlink r:id="rId248" ref="D121"/>
+    <hyperlink r:id="rId249" ref="E121"/>
+    <hyperlink r:id="rId250" ref="F121"/>
+    <hyperlink r:id="rId251" ref="D122"/>
+    <hyperlink r:id="rId252" ref="E122"/>
+    <hyperlink r:id="rId253" ref="D123"/>
+    <hyperlink r:id="rId254" ref="E123"/>
+    <hyperlink r:id="rId255" ref="F123"/>
+    <hyperlink r:id="rId256" ref="D124"/>
+    <hyperlink r:id="rId257" ref="E124"/>
+    <hyperlink r:id="rId258" ref="D125"/>
+    <hyperlink r:id="rId259" ref="E125"/>
+    <hyperlink r:id="rId260" ref="D126"/>
+    <hyperlink r:id="rId261" ref="E126"/>
+    <hyperlink r:id="rId262" ref="D127"/>
+    <hyperlink r:id="rId263" ref="E127"/>
   </hyperlinks>
-  <drawing r:id="rId260"/>
+  <drawing r:id="rId264"/>
 </worksheet>
 </file>
 
@@ -14610,7 +14663,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="69" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="G1" s="72"/>
       <c r="H1" s="72"/>
@@ -14635,27 +14688,27 @@
     </row>
     <row r="2">
       <c r="A2" s="73" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="B2" s="74">
         <v>3.0</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="D2" s="76" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="E2" s="77" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="F2" s="74" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="73" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="B3" s="78">
         <v>45353.0</v>
@@ -14664,16 +14717,16 @@
         <v>9</v>
       </c>
       <c r="D3" s="77" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="F3" s="80"/>
     </row>
     <row r="4">
       <c r="A4" s="73" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="B4" s="74">
         <v>3.0</v>
@@ -14682,16 +14735,16 @@
         <v>9</v>
       </c>
       <c r="D4" s="76" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="E4" s="76" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="F4" s="80"/>
     </row>
     <row r="5">
       <c r="A5" s="73" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="B5" s="74">
         <v>3.0</v>
@@ -14700,38 +14753,38 @@
         <v>9</v>
       </c>
       <c r="D5" s="76" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="E5" s="81" t="s">
         <v>30</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="73" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="B6" s="74">
         <v>3.0</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="D6" s="77" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="E6" s="77" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="F6" s="74" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="73" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="B7" s="74">
         <v>3.0</v>
@@ -14740,13 +14793,13 @@
         <v>9</v>
       </c>
       <c r="D7" s="76" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="E7" s="76" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8">
@@ -22729,22 +22782,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="84" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="E1" s="71" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="69" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="G1" s="72"/>
       <c r="H1" s="72"/>
@@ -22769,22 +22822,22 @@
     </row>
     <row r="2">
       <c r="A2" s="85" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="B2" s="85" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="C2" s="85" t="s">
         <v>55</v>
       </c>
       <c r="D2" s="85" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="E2" s="86" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="F2" s="85" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="G2" s="87"/>
       <c r="H2" s="87"/>
@@ -22977,7 +23030,7 @@
     </row>
     <row r="9">
       <c r="A9" s="85" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="B9" s="87"/>
       <c r="C9" s="87"/>
@@ -23007,7 +23060,7 @@
     </row>
     <row r="10">
       <c r="A10" s="89" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="B10" s="87"/>
       <c r="C10" s="87"/>
@@ -26556,75 +26609,75 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="84" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="E1" s="71" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="69" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="91" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="B2" s="92"/>
       <c r="C2" s="91" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="D2" s="93">
         <v>45746.0</v>
       </c>
       <c r="E2" s="94" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="F2" s="95" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="91" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="B3" s="96">
         <v>4.0</v>
       </c>
       <c r="C3" s="95" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="D3" s="93">
         <v>45899.0</v>
       </c>
       <c r="E3" s="94" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="F3" s="91" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="91" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="B4" s="92"/>
       <c r="D4" s="93">
         <v>45884.0</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="F4" s="95" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
     </row>
     <row r="5">
@@ -30641,10 +30694,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="C1" s="97" t="s">
         <v>3</v>
@@ -30677,89 +30730,89 @@
     </row>
     <row r="2">
       <c r="A2" s="99" t="s">
-        <v>529</v>
+        <v>534</v>
       </c>
       <c r="B2" s="96" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
       <c r="D2" s="100"/>
       <c r="E2" s="101"/>
     </row>
     <row r="3">
       <c r="A3" s="99" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="B3" s="96" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="D3" s="100"/>
       <c r="E3" s="101"/>
     </row>
     <row r="4">
       <c r="A4" s="99" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="B4" s="96">
         <v>2024.0</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="D4" s="100"/>
       <c r="E4" s="101"/>
     </row>
     <row r="5">
       <c r="A5" s="99" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="B5" s="96" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="D5" s="100"/>
       <c r="E5" s="101"/>
     </row>
     <row r="6">
       <c r="A6" s="99" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="B6" s="96">
         <v>2025.0</v>
       </c>
       <c r="C6" s="100" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="D6" s="100"/>
       <c r="E6" s="101"/>
     </row>
     <row r="7">
       <c r="A7" s="99" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="B7" s="96" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="102" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="B8" s="96">
         <v>2025.0</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>544</v>
+        <v>549</v>
       </c>
     </row>
     <row r="9">
@@ -34760,82 +34813,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="104" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="B1" s="104" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="105" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="B2" s="105" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="105" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="105" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="105" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="105" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="105" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="105" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="B8" s="105" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="105" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="B9" s="105" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="105" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="B10" s="105" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Added several Q1/Q2 journals
</commit_message>
<xml_diff>
--- a/source/Journals.xlsx
+++ b/source/Journals.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="589">
   <si>
     <t>Journal</t>
   </si>
@@ -1241,6 +1241,60 @@
   </si>
   <si>
     <t>First decision &lt;= 6 days, time to publish: 178 days</t>
+  </si>
+  <si>
+    <t>International Journal of System Assurance Engineering and Management</t>
+  </si>
+  <si>
+    <t>https://www.scimagojr.com/journalsearch.php?q=19700177002&amp;tip=sid&amp;clean=0</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s13198-025-02913-2</t>
+  </si>
+  <si>
+    <t>First decision &lt;= 93 days</t>
+  </si>
+  <si>
+    <t>Scientific Reports</t>
+  </si>
+  <si>
+    <t>2690 USD</t>
+  </si>
+  <si>
+    <t>https://www.scimagojr.com/journalsearch.php?q=21100200805&amp;tip=sid</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41598-025-07915-5</t>
+  </si>
+  <si>
+    <t>Nature! First decision &lt;= 21 days, time to publish: 137 days</t>
+  </si>
+  <si>
+    <t>Mathematical Problems in Engineering</t>
+  </si>
+  <si>
+    <t>https://www.scimagojr.com/journalsearch.php?q=13082&amp;tip=sid&amp;clean=0</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1155/2021/9949999</t>
+  </si>
+  <si>
+    <t>time to publish &gt;= 60 days</t>
+  </si>
+  <si>
+    <t>Demonstratio Mathematica</t>
+  </si>
+  <si>
+    <t>1050 USD</t>
+  </si>
+  <si>
+    <t>https://www.scimagojr.com/journalsearch.php?q=21100836176&amp;tip=sid&amp;clean=0</t>
+  </si>
+  <si>
+    <t>https://www.degruyterbrill.com/search/series/dema?query=Survival+analysis&amp;documentVisibility=all</t>
+  </si>
+  <si>
+    <t>Publication Frequency: 1 issue per year?</t>
   </si>
   <si>
     <t>Decision Sciences</t>
@@ -4627,167 +4681,167 @@
       <c r="G76" s="12"/>
     </row>
     <row r="77">
-      <c r="A77" s="7"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="27"/>
+      <c r="A77" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C77" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="F77" s="27" t="s">
+        <v>325</v>
+      </c>
       <c r="G77" s="12"/>
     </row>
     <row r="78">
-      <c r="A78" s="43" t="s">
-        <v>322</v>
-      </c>
-      <c r="B78" s="44"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="46"/>
-      <c r="E78" s="47"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="48"/>
+      <c r="A78" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="F78" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="G78" s="12"/>
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="25" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="F79" s="27" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="G79" s="12"/>
     </row>
     <row r="80">
-      <c r="A80" s="7"/>
-      <c r="B80" s="8"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="30"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="27"/>
+      <c r="A80" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="F80" s="27" t="s">
+        <v>339</v>
+      </c>
       <c r="G80" s="12"/>
     </row>
     <row r="81">
-      <c r="A81" s="43" t="s">
-        <v>327</v>
-      </c>
-      <c r="B81" s="44"/>
-      <c r="C81" s="45"/>
-      <c r="D81" s="46"/>
-      <c r="E81" s="47"/>
-      <c r="F81" s="45"/>
-      <c r="G81" s="48"/>
+      <c r="A81" s="7"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="12"/>
     </row>
     <row r="82">
-      <c r="A82" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="B82" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="D82" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="E82" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="F82" s="9"/>
-      <c r="G82" s="12"/>
+      <c r="A82" s="43" t="s">
+        <v>340</v>
+      </c>
+      <c r="B82" s="44"/>
+      <c r="C82" s="45"/>
+      <c r="D82" s="46"/>
+      <c r="E82" s="47"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="48"/>
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="B83" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B83" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C83" s="49" t="s">
+      <c r="C83" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D83" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="E83" s="15" t="s">
-        <v>334</v>
-      </c>
-      <c r="F83" s="11" t="s">
-        <v>335</v>
+      <c r="D83" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="F83" s="27" t="s">
+        <v>344</v>
       </c>
       <c r="G83" s="12"/>
     </row>
     <row r="84">
-      <c r="A84" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="D84" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="E84" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="F84" s="25" t="s">
-        <v>340</v>
-      </c>
+      <c r="A84" s="7"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="30"/>
+      <c r="F84" s="27"/>
       <c r="G84" s="12"/>
     </row>
     <row r="85">
-      <c r="A85" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D85" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="E85" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="F85" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="G85" s="12"/>
+      <c r="A85" s="43" t="s">
+        <v>345</v>
+      </c>
+      <c r="B85" s="44"/>
+      <c r="C85" s="45"/>
+      <c r="D85" s="46"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="45"/>
+      <c r="G85" s="48"/>
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="B86" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B86" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C86" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="D86" s="16" t="s">
+      <c r="C86" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="E86" s="24" t="s">
+      <c r="D86" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="F86" s="11" t="s">
+      <c r="E86" s="15" t="s">
         <v>349</v>
       </c>
+      <c r="F86" s="9"/>
       <c r="G86" s="12"/>
     </row>
     <row r="87">
@@ -4797,8 +4851,8 @@
       <c r="B87" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C87" s="9" t="s">
-        <v>50</v>
+      <c r="C87" s="49" t="s">
+        <v>9</v>
       </c>
       <c r="D87" s="15" t="s">
         <v>351</v>
@@ -4815,19 +4869,19 @@
       <c r="A88" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="B88" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C88" s="11" t="s">
+      <c r="B88" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="D88" s="10" t="s">
+      <c r="D88" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="E88" s="10" t="s">
+      <c r="E88" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="F88" s="50" t="s">
+      <c r="F88" s="25" t="s">
         <v>358</v>
       </c>
       <c r="G88" s="12"/>
@@ -4840,7 +4894,7 @@
         <v>8</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D89" s="15" t="s">
         <v>360</v>
@@ -4854,64 +4908,64 @@
       <c r="G89" s="12"/>
     </row>
     <row r="90">
-      <c r="A90" s="51" t="s">
+      <c r="A90" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="B90" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D90" s="15" t="s">
+      <c r="B90" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="E90" s="15" t="s">
+      <c r="D90" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="F90" s="9" t="s">
+      <c r="E90" s="24" t="s">
         <v>366</v>
       </c>
+      <c r="F90" s="11" t="s">
+        <v>367</v>
+      </c>
       <c r="G90" s="12"/>
     </row>
     <row r="91">
-      <c r="A91" s="52" t="s">
-        <v>367</v>
-      </c>
-      <c r="B91" s="8" t="s">
+      <c r="A91" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B91" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C91" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="D91" s="10" t="s">
+      <c r="C91" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D91" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="E91" s="30" t="s">
+      <c r="E91" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="F91" s="25" t="s">
+      <c r="F91" s="11" t="s">
         <v>371</v>
       </c>
       <c r="G91" s="12"/>
     </row>
     <row r="92">
-      <c r="A92" s="53" t="s">
+      <c r="A92" s="7" t="s">
         <v>372</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C92" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="D92" s="16" t="s">
+      <c r="D92" s="10" t="s">
         <v>374</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="F92" s="25" t="s">
+      <c r="F92" s="50" t="s">
         <v>376</v>
       </c>
       <c r="G92" s="12"/>
@@ -4920,672 +4974,720 @@
       <c r="A93" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="B93" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="E93" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="G93" s="12"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="B94" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="C93" s="11" t="s">
-        <v>378</v>
-      </c>
-      <c r="D93" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="E93" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="F93" s="27" t="s">
-        <v>381</v>
-      </c>
-      <c r="G93" s="12"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>8</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D94" s="10" t="s">
+      <c r="D94" s="15" t="s">
+        <v>382</v>
+      </c>
+      <c r="E94" s="15" t="s">
         <v>383</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="F94" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="F94" s="27" t="s">
-        <v>278</v>
-      </c>
       <c r="G94" s="12"/>
     </row>
     <row r="95">
-      <c r="A95" s="7" t="s">
+      <c r="A95" s="52" t="s">
         <v>385</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="25" t="s">
-        <v>182</v>
+      <c r="C95" s="11" t="s">
+        <v>386</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>386</v>
-      </c>
-      <c r="E95" s="10" t="s">
         <v>387</v>
       </c>
+      <c r="E95" s="30" t="s">
+        <v>388</v>
+      </c>
       <c r="F95" s="25" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="G95" s="12"/>
     </row>
     <row r="96">
-      <c r="A96" s="28" t="s">
-        <v>389</v>
+      <c r="A96" s="53" t="s">
+        <v>390</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C96" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="D96" s="10" t="s">
+      <c r="C96" s="11" t="s">
         <v>391</v>
       </c>
+      <c r="D96" s="16" t="s">
+        <v>392</v>
+      </c>
       <c r="E96" s="10" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F96" s="25" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G96" s="12"/>
     </row>
     <row r="97">
-      <c r="A97" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="B97" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D97" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="E97" s="57" t="s">
-        <v>394</v>
-      </c>
-      <c r="F97" s="54" t="s">
-        <v>236</v>
-      </c>
-      <c r="G97" s="58"/>
+      <c r="A97" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="F97" s="27" t="s">
+        <v>399</v>
+      </c>
+      <c r="G97" s="12"/>
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C98" s="25" t="s">
+      <c r="C98" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="F98" s="27" t="s">
-        <v>398</v>
+        <v>278</v>
       </c>
       <c r="G98" s="12"/>
     </row>
     <row r="99">
-      <c r="A99" s="59"/>
-      <c r="B99" s="60"/>
-      <c r="C99" s="59"/>
-      <c r="D99" s="60"/>
-      <c r="E99" s="61"/>
-      <c r="F99" s="59"/>
-      <c r="G99" s="41"/>
+      <c r="A99" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="F99" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="G99" s="12"/>
     </row>
     <row r="100">
-      <c r="A100" s="43" t="s">
-        <v>399</v>
-      </c>
-      <c r="B100" s="44"/>
-      <c r="C100" s="45"/>
-      <c r="D100" s="46"/>
-      <c r="E100" s="47"/>
-      <c r="F100" s="45"/>
-      <c r="G100" s="48"/>
+      <c r="A100" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="F100" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="G100" s="12"/>
     </row>
     <row r="101">
-      <c r="A101" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="B101" s="8" t="s">
+      <c r="A101" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C101" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="E101" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="F101" s="27"/>
-      <c r="G101" s="12"/>
+      <c r="C101" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E101" s="57" t="s">
+        <v>412</v>
+      </c>
+      <c r="F101" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="G101" s="58"/>
     </row>
     <row r="102">
-      <c r="A102" s="7"/>
-      <c r="B102" s="8"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="30"/>
-      <c r="E102" s="30"/>
-      <c r="F102" s="27"/>
+      <c r="A102" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="F102" s="27" t="s">
+        <v>416</v>
+      </c>
       <c r="G102" s="12"/>
     </row>
     <row r="103">
-      <c r="A103" s="43" t="s">
-        <v>403</v>
-      </c>
-      <c r="B103" s="44"/>
-      <c r="C103" s="45"/>
-      <c r="D103" s="46" t="s">
-        <v>404</v>
-      </c>
-      <c r="E103" s="47"/>
-      <c r="F103" s="45"/>
-      <c r="G103" s="48"/>
+      <c r="A103" s="59"/>
+      <c r="B103" s="60"/>
+      <c r="C103" s="59"/>
+      <c r="D103" s="60"/>
+      <c r="E103" s="61"/>
+      <c r="F103" s="59"/>
+      <c r="G103" s="41"/>
     </row>
     <row r="104">
-      <c r="A104" s="28" t="s">
-        <v>405</v>
-      </c>
-      <c r="B104" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="E104" s="26" t="s">
-        <v>407</v>
-      </c>
-      <c r="F104" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="G104" s="12"/>
+      <c r="A104" s="43" t="s">
+        <v>417</v>
+      </c>
+      <c r="B104" s="44"/>
+      <c r="C104" s="45"/>
+      <c r="D104" s="46"/>
+      <c r="E104" s="47"/>
+      <c r="F104" s="45"/>
+      <c r="G104" s="48"/>
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>410</v>
+        <v>30</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="E105" s="62" t="s">
+        <v>419</v>
+      </c>
+      <c r="E105" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="F105" s="27"/>
+      <c r="G105" s="12"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="7"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="30"/>
+      <c r="E106" s="30"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="12"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="43" t="s">
+        <v>421</v>
+      </c>
+      <c r="B107" s="44"/>
+      <c r="C107" s="45"/>
+      <c r="D107" s="46" t="s">
+        <v>422</v>
+      </c>
+      <c r="E107" s="47"/>
+      <c r="F107" s="45"/>
+      <c r="G107" s="48"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="28" t="s">
+        <v>423</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="D108" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="E108" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="F108" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="G108" s="12"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="D109" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="E109" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="F105" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="G105" s="12"/>
-    </row>
-    <row r="106">
-      <c r="A106" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="B106" s="8" t="s">
+      <c r="F109" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="G109" s="12"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C106" s="9" t="s">
+      <c r="C110" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D106" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="E106" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="F106" s="25" t="s">
-        <v>416</v>
-      </c>
-      <c r="G106" s="12"/>
-    </row>
-    <row r="107">
-      <c r="A107" s="28" t="s">
-        <v>417</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C107" s="25" t="s">
-        <v>418</v>
-      </c>
-      <c r="D107" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="E107" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="F107" s="27" t="s">
-        <v>421</v>
-      </c>
-      <c r="G107" s="12"/>
-    </row>
-    <row r="108">
-      <c r="A108" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D108" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="E108" s="63" t="s">
-        <v>424</v>
-      </c>
-      <c r="F108" s="25" t="s">
-        <v>425</v>
-      </c>
-      <c r="G108" s="12"/>
-    </row>
-    <row r="109">
-      <c r="A109" s="13"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="9"/>
-      <c r="D109" s="64"/>
-      <c r="E109" s="64"/>
-      <c r="F109" s="9"/>
-      <c r="G109" s="12"/>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B110" s="44"/>
-      <c r="C110" s="45"/>
-      <c r="D110" s="65" t="s">
-        <v>427</v>
-      </c>
-      <c r="E110" s="47"/>
-      <c r="F110" s="45"/>
-      <c r="G110" s="48"/>
+      <c r="D110" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="E110" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="F110" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="G110" s="12"/>
     </row>
     <row r="111">
-      <c r="A111" s="7" t="s">
-        <v>428</v>
+      <c r="A111" s="28" t="s">
+        <v>435</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C111" s="9" t="s">
+      <c r="C111" s="25" t="s">
+        <v>436</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="E111" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="F111" s="27" t="s">
+        <v>439</v>
+      </c>
+      <c r="G111" s="12"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C112" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D111" s="16" t="s">
-        <v>429</v>
-      </c>
-      <c r="E111" s="26" t="s">
-        <v>430</v>
-      </c>
-      <c r="F111" s="11" t="s">
-        <v>431</v>
-      </c>
-      <c r="G111" s="12"/>
-    </row>
-    <row r="112">
-      <c r="A112" s="13" t="s">
-        <v>432</v>
-      </c>
-      <c r="B112" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C112" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="D112" s="15" t="s">
-        <v>434</v>
-      </c>
-      <c r="E112" s="64" t="s">
-        <v>435</v>
-      </c>
-      <c r="F112" s="9" t="s">
-        <v>436</v>
+      <c r="D112" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="E112" s="63" t="s">
+        <v>442</v>
+      </c>
+      <c r="F112" s="25" t="s">
+        <v>443</v>
       </c>
       <c r="G112" s="12"/>
     </row>
     <row r="113">
-      <c r="A113" s="13" t="s">
-        <v>437</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>438</v>
-      </c>
-      <c r="D113" s="15" t="s">
-        <v>439</v>
-      </c>
-      <c r="E113" s="64" t="s">
-        <v>435</v>
-      </c>
+      <c r="A113" s="13"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="64"/>
+      <c r="E113" s="64"/>
       <c r="F113" s="9"/>
       <c r="G113" s="12"/>
     </row>
     <row r="114">
-      <c r="A114" s="13" t="s">
-        <v>440</v>
-      </c>
-      <c r="B114" s="14" t="s">
+      <c r="A114" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B114" s="44"/>
+      <c r="C114" s="45"/>
+      <c r="D114" s="65" t="s">
+        <v>445</v>
+      </c>
+      <c r="E114" s="47"/>
+      <c r="F114" s="45"/>
+      <c r="G114" s="48"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="B115" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C114" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="D114" s="15" t="s">
-        <v>442</v>
-      </c>
-      <c r="E114" s="15" t="s">
-        <v>443</v>
-      </c>
-      <c r="F114" s="9"/>
-      <c r="G114" s="12"/>
-    </row>
-    <row r="115">
-      <c r="A115" s="13" t="s">
-        <v>444</v>
-      </c>
-      <c r="B115" s="14" t="s">
-        <v>37</v>
-      </c>
       <c r="C115" s="9" t="s">
-        <v>445</v>
-      </c>
-      <c r="D115" s="15" t="s">
-        <v>446</v>
-      </c>
-      <c r="E115" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" s="16" t="s">
         <v>447</v>
       </c>
-      <c r="F115" s="9"/>
+      <c r="E115" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="F115" s="11" t="s">
+        <v>449</v>
+      </c>
       <c r="G115" s="12"/>
     </row>
     <row r="116">
       <c r="A116" s="13" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="D116" s="15" t="s">
-        <v>449</v>
-      </c>
-      <c r="E116" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="F116" s="9"/>
+        <v>452</v>
+      </c>
+      <c r="E116" s="64" t="s">
+        <v>453</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>454</v>
+      </c>
       <c r="G116" s="12"/>
     </row>
     <row r="117">
       <c r="A117" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="B117" s="14" t="s">
-        <v>37</v>
+        <v>455</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>445</v>
+        <v>456</v>
       </c>
       <c r="D117" s="15" t="s">
-        <v>452</v>
-      </c>
-      <c r="E117" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="E117" s="64" t="s">
         <v>453</v>
       </c>
       <c r="F117" s="9"/>
       <c r="G117" s="12"/>
     </row>
     <row r="118">
-      <c r="A118" s="7" t="s">
-        <v>454</v>
-      </c>
-      <c r="B118" s="8" t="s">
+      <c r="A118" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="B118" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="D118" s="10" t="s">
-        <v>455</v>
-      </c>
-      <c r="E118" s="10" t="s">
-        <v>456</v>
+        <v>459</v>
+      </c>
+      <c r="D118" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="E118" s="15" t="s">
+        <v>461</v>
       </c>
       <c r="F118" s="9"/>
       <c r="G118" s="12"/>
     </row>
     <row r="119">
-      <c r="A119" s="7" t="s">
-        <v>457</v>
-      </c>
-      <c r="B119" s="8" t="s">
+      <c r="A119" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="B119" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C119" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="D119" s="10" t="s">
-        <v>459</v>
-      </c>
-      <c r="E119" s="24" t="s">
-        <v>460</v>
+      <c r="C119" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="D119" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="E119" s="66" t="s">
+        <v>465</v>
       </c>
       <c r="F119" s="9"/>
       <c r="G119" s="12"/>
     </row>
     <row r="120">
-      <c r="A120" s="7" t="s">
-        <v>461</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C120" s="11" t="s">
-        <v>445</v>
-      </c>
-      <c r="D120" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="E120" s="10" t="s">
+      <c r="A120" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" s="9" t="s">
         <v>463</v>
+      </c>
+      <c r="D120" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="E120" s="15" t="s">
+        <v>468</v>
       </c>
       <c r="F120" s="9"/>
       <c r="G120" s="12"/>
     </row>
     <row r="121">
-      <c r="A121" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="B121" s="8" t="s">
+      <c r="A121" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="B121" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C121" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="D121" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="E121" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="F121" s="25" t="s">
-        <v>467</v>
-      </c>
+      <c r="C121" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="D121" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="E121" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="F121" s="9"/>
       <c r="G121" s="12"/>
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C122" s="11" t="s">
-        <v>469</v>
+      <c r="C122" s="9" t="s">
+        <v>459</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="E122" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="F122" s="27"/>
+        <v>474</v>
+      </c>
+      <c r="F122" s="9"/>
       <c r="G122" s="12"/>
     </row>
     <row r="123">
       <c r="A123" s="7" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="D123" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="E123" s="10" t="s">
-        <v>475</v>
-      </c>
-      <c r="F123" s="25" t="s">
-        <v>476</v>
-      </c>
+        <v>477</v>
+      </c>
+      <c r="E123" s="24" t="s">
+        <v>478</v>
+      </c>
+      <c r="F123" s="9"/>
       <c r="G123" s="12"/>
     </row>
     <row r="124">
       <c r="A124" s="7" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B124" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C124" s="9" t="s">
-        <v>441</v>
+      <c r="C124" s="11" t="s">
+        <v>463</v>
       </c>
       <c r="D124" s="10" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E124" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="F124" s="27"/>
+        <v>481</v>
+      </c>
+      <c r="F124" s="9"/>
       <c r="G124" s="12"/>
     </row>
     <row r="125">
-      <c r="A125" s="13" t="s">
-        <v>480</v>
-      </c>
-      <c r="B125" s="14" t="s">
+      <c r="A125" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="D125" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="E125" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="F125" s="25" t="s">
+        <v>485</v>
+      </c>
+      <c r="G125" s="12"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="D126" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="E126" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="F126" s="27"/>
+      <c r="G126" s="12"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="B127" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C125" s="9" t="s">
+      <c r="C127" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="D127" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E127" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="F127" s="25" t="s">
+        <v>494</v>
+      </c>
+      <c r="G127" s="12"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="D128" s="10" t="s">
+        <v>496</v>
+      </c>
+      <c r="E128" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="F128" s="27"/>
+      <c r="G128" s="12"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C129" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D125" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="E125" s="15" t="s">
+      <c r="D129" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="E129" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F125" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="G125" s="12"/>
-    </row>
-    <row r="126">
-      <c r="A126" s="53" t="s">
-        <v>483</v>
-      </c>
-      <c r="B126" s="8" t="s">
+      <c r="F129" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="G129" s="12"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="53" t="s">
+        <v>501</v>
+      </c>
+      <c r="B130" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C126" s="11" t="s">
+      <c r="C130" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D126" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="E126" s="10" t="s">
-        <v>485</v>
-      </c>
-      <c r="F126" s="27" t="s">
-        <v>486</v>
-      </c>
-      <c r="G126" s="12"/>
-    </row>
-    <row r="127">
-      <c r="A127" s="13"/>
-      <c r="B127" s="14"/>
-      <c r="C127" s="9"/>
-      <c r="D127" s="64"/>
-      <c r="E127" s="64"/>
-      <c r="F127" s="9"/>
-      <c r="G127" s="12"/>
-    </row>
-    <row r="128">
-      <c r="A128" s="13"/>
-      <c r="B128" s="14"/>
-      <c r="C128" s="9"/>
-      <c r="D128" s="64"/>
-      <c r="E128" s="64"/>
-      <c r="F128" s="9"/>
-      <c r="G128" s="12"/>
-    </row>
-    <row r="129">
-      <c r="A129" s="13"/>
-      <c r="B129" s="14"/>
-      <c r="C129" s="27"/>
-      <c r="D129" s="64"/>
-      <c r="E129" s="64"/>
-      <c r="F129" s="9"/>
-      <c r="G129" s="12"/>
-    </row>
-    <row r="130">
-      <c r="A130" s="13"/>
-      <c r="B130" s="14"/>
-      <c r="C130" s="11"/>
-      <c r="D130" s="64"/>
-      <c r="E130" s="64"/>
-      <c r="F130" s="9"/>
+      <c r="D130" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="E130" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="F130" s="27" t="s">
+        <v>504</v>
+      </c>
       <c r="G130" s="12"/>
     </row>
     <row r="131">
       <c r="A131" s="13"/>
       <c r="B131" s="14"/>
-      <c r="C131" s="11"/>
+      <c r="C131" s="9"/>
       <c r="D131" s="64"/>
       <c r="E131" s="64"/>
       <c r="F131" s="9"/>
@@ -5594,7 +5696,7 @@
     <row r="132">
       <c r="A132" s="13"/>
       <c r="B132" s="14"/>
-      <c r="C132" s="11"/>
+      <c r="C132" s="9"/>
       <c r="D132" s="64"/>
       <c r="E132" s="64"/>
       <c r="F132" s="9"/>
@@ -5603,7 +5705,7 @@
     <row r="133">
       <c r="A133" s="13"/>
       <c r="B133" s="14"/>
-      <c r="C133" s="11"/>
+      <c r="C133" s="27"/>
       <c r="D133" s="64"/>
       <c r="E133" s="64"/>
       <c r="F133" s="9"/>
@@ -5611,7 +5713,7 @@
     </row>
     <row r="134">
       <c r="A134" s="13"/>
-      <c r="B134" s="67"/>
+      <c r="B134" s="14"/>
       <c r="C134" s="11"/>
       <c r="D134" s="64"/>
       <c r="E134" s="64"/>
@@ -5630,7 +5732,7 @@
     <row r="136">
       <c r="A136" s="13"/>
       <c r="B136" s="14"/>
-      <c r="C136" s="9"/>
+      <c r="C136" s="11"/>
       <c r="D136" s="64"/>
       <c r="E136" s="64"/>
       <c r="F136" s="9"/>
@@ -5639,7 +5741,7 @@
     <row r="137">
       <c r="A137" s="13"/>
       <c r="B137" s="14"/>
-      <c r="C137" s="9"/>
+      <c r="C137" s="11"/>
       <c r="D137" s="64"/>
       <c r="E137" s="64"/>
       <c r="F137" s="9"/>
@@ -5647,8 +5749,8 @@
     </row>
     <row r="138">
       <c r="A138" s="13"/>
-      <c r="B138" s="14"/>
-      <c r="C138" s="9"/>
+      <c r="B138" s="67"/>
+      <c r="C138" s="11"/>
       <c r="D138" s="64"/>
       <c r="E138" s="64"/>
       <c r="F138" s="9"/>
@@ -5657,7 +5759,7 @@
     <row r="139">
       <c r="A139" s="13"/>
       <c r="B139" s="14"/>
-      <c r="C139" s="9"/>
+      <c r="C139" s="11"/>
       <c r="D139" s="64"/>
       <c r="E139" s="64"/>
       <c r="F139" s="9"/>
@@ -14356,6 +14458,42 @@
       <c r="E1105" s="64"/>
       <c r="F1105" s="9"/>
       <c r="G1105" s="12"/>
+    </row>
+    <row r="1106">
+      <c r="A1106" s="13"/>
+      <c r="B1106" s="14"/>
+      <c r="C1106" s="9"/>
+      <c r="D1106" s="64"/>
+      <c r="E1106" s="64"/>
+      <c r="F1106" s="9"/>
+      <c r="G1106" s="12"/>
+    </row>
+    <row r="1107">
+      <c r="A1107" s="13"/>
+      <c r="B1107" s="14"/>
+      <c r="C1107" s="9"/>
+      <c r="D1107" s="64"/>
+      <c r="E1107" s="64"/>
+      <c r="F1107" s="9"/>
+      <c r="G1107" s="12"/>
+    </row>
+    <row r="1108">
+      <c r="A1108" s="13"/>
+      <c r="B1108" s="14"/>
+      <c r="C1108" s="9"/>
+      <c r="D1108" s="64"/>
+      <c r="E1108" s="64"/>
+      <c r="F1108" s="9"/>
+      <c r="G1108" s="12"/>
+    </row>
+    <row r="1109">
+      <c r="A1109" s="13"/>
+      <c r="B1109" s="14"/>
+      <c r="C1109" s="9"/>
+      <c r="D1109" s="64"/>
+      <c r="E1109" s="64"/>
+      <c r="F1109" s="9"/>
+      <c r="G1109" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -14529,100 +14667,111 @@
     <hyperlink r:id="rId168" ref="C76"/>
     <hyperlink r:id="rId169" ref="D76"/>
     <hyperlink r:id="rId170" ref="E76"/>
-    <hyperlink r:id="rId171" location="aims-and-scope" ref="C79"/>
-    <hyperlink r:id="rId172" ref="D79"/>
-    <hyperlink r:id="rId173" ref="E79"/>
-    <hyperlink r:id="rId174" ref="D82"/>
-    <hyperlink r:id="rId175" ref="E82"/>
-    <hyperlink r:id="rId176" ref="D83"/>
-    <hyperlink r:id="rId177" ref="E83"/>
-    <hyperlink r:id="rId178" ref="D84"/>
-    <hyperlink r:id="rId179" ref="E84"/>
-    <hyperlink r:id="rId180" ref="F84"/>
-    <hyperlink r:id="rId181" ref="D85"/>
-    <hyperlink r:id="rId182" ref="E85"/>
-    <hyperlink r:id="rId183" ref="D86"/>
-    <hyperlink r:id="rId184" ref="E86"/>
-    <hyperlink r:id="rId185" ref="D87"/>
-    <hyperlink r:id="rId186" ref="E87"/>
-    <hyperlink r:id="rId187" ref="D88"/>
-    <hyperlink r:id="rId188" ref="E88"/>
-    <hyperlink r:id="rId189" ref="D89"/>
-    <hyperlink r:id="rId190" ref="E89"/>
-    <hyperlink r:id="rId191" location="callForPapersHeader" ref="D90"/>
-    <hyperlink r:id="rId192" ref="E90"/>
-    <hyperlink r:id="rId193" ref="D91"/>
-    <hyperlink r:id="rId194" ref="F91"/>
-    <hyperlink r:id="rId195" ref="D92"/>
-    <hyperlink r:id="rId196" ref="E92"/>
-    <hyperlink r:id="rId197" ref="F92"/>
-    <hyperlink r:id="rId198" ref="D93"/>
-    <hyperlink r:id="rId199" ref="E93"/>
-    <hyperlink r:id="rId200" ref="D94"/>
-    <hyperlink r:id="rId201" ref="E94"/>
-    <hyperlink r:id="rId202" ref="C95"/>
-    <hyperlink r:id="rId203" ref="D95"/>
-    <hyperlink r:id="rId204" ref="E95"/>
+    <hyperlink r:id="rId171" ref="C77"/>
+    <hyperlink r:id="rId172" ref="D77"/>
+    <hyperlink r:id="rId173" ref="E77"/>
+    <hyperlink r:id="rId174" ref="C78"/>
+    <hyperlink r:id="rId175" ref="D78"/>
+    <hyperlink r:id="rId176" ref="E78"/>
+    <hyperlink r:id="rId177" ref="F78"/>
+    <hyperlink r:id="rId178" ref="D79"/>
+    <hyperlink r:id="rId179" ref="E79"/>
+    <hyperlink r:id="rId180" ref="D80"/>
+    <hyperlink r:id="rId181" ref="E80"/>
+    <hyperlink r:id="rId182" location="aims-and-scope" ref="C83"/>
+    <hyperlink r:id="rId183" ref="D83"/>
+    <hyperlink r:id="rId184" ref="E83"/>
+    <hyperlink r:id="rId185" ref="D86"/>
+    <hyperlink r:id="rId186" ref="E86"/>
+    <hyperlink r:id="rId187" ref="D87"/>
+    <hyperlink r:id="rId188" ref="E87"/>
+    <hyperlink r:id="rId189" ref="D88"/>
+    <hyperlink r:id="rId190" ref="E88"/>
+    <hyperlink r:id="rId191" ref="F88"/>
+    <hyperlink r:id="rId192" ref="D89"/>
+    <hyperlink r:id="rId193" ref="E89"/>
+    <hyperlink r:id="rId194" ref="D90"/>
+    <hyperlink r:id="rId195" ref="E90"/>
+    <hyperlink r:id="rId196" ref="D91"/>
+    <hyperlink r:id="rId197" ref="E91"/>
+    <hyperlink r:id="rId198" ref="D92"/>
+    <hyperlink r:id="rId199" ref="E92"/>
+    <hyperlink r:id="rId200" ref="D93"/>
+    <hyperlink r:id="rId201" ref="E93"/>
+    <hyperlink r:id="rId202" location="callForPapersHeader" ref="D94"/>
+    <hyperlink r:id="rId203" ref="E94"/>
+    <hyperlink r:id="rId204" ref="D95"/>
     <hyperlink r:id="rId205" ref="F95"/>
-    <hyperlink r:id="rId206" ref="C96"/>
-    <hyperlink r:id="rId207" ref="D96"/>
-    <hyperlink r:id="rId208" ref="E96"/>
-    <hyperlink r:id="rId209" ref="F96"/>
-    <hyperlink r:id="rId210" ref="D97"/>
-    <hyperlink r:id="rId211" ref="E97"/>
-    <hyperlink r:id="rId212" ref="C98"/>
-    <hyperlink r:id="rId213" ref="D98"/>
-    <hyperlink r:id="rId214" ref="E98"/>
-    <hyperlink r:id="rId215" ref="D101"/>
-    <hyperlink r:id="rId216" ref="E101"/>
-    <hyperlink r:id="rId217" ref="D103"/>
-    <hyperlink r:id="rId218" ref="D104"/>
-    <hyperlink r:id="rId219" ref="E104"/>
-    <hyperlink r:id="rId220" ref="D105"/>
-    <hyperlink r:id="rId221" ref="D106"/>
-    <hyperlink r:id="rId222" ref="E106"/>
-    <hyperlink r:id="rId223" ref="F106"/>
-    <hyperlink r:id="rId224" ref="C107"/>
-    <hyperlink r:id="rId225" ref="D107"/>
-    <hyperlink r:id="rId226" ref="E107"/>
-    <hyperlink r:id="rId227" ref="D108"/>
-    <hyperlink r:id="rId228" ref="E108"/>
-    <hyperlink r:id="rId229" ref="F108"/>
-    <hyperlink r:id="rId230" ref="D110"/>
-    <hyperlink r:id="rId231" ref="D111"/>
-    <hyperlink r:id="rId232" ref="E111"/>
-    <hyperlink r:id="rId233" ref="D112"/>
-    <hyperlink r:id="rId234" ref="D113"/>
-    <hyperlink r:id="rId235" ref="D114"/>
-    <hyperlink r:id="rId236" ref="E114"/>
-    <hyperlink r:id="rId237" ref="D115"/>
-    <hyperlink r:id="rId238" ref="E115"/>
-    <hyperlink r:id="rId239" ref="D116"/>
-    <hyperlink r:id="rId240" ref="E116"/>
-    <hyperlink r:id="rId241" ref="D117"/>
-    <hyperlink r:id="rId242" ref="E117"/>
-    <hyperlink r:id="rId243" ref="D118"/>
-    <hyperlink r:id="rId244" ref="E118"/>
-    <hyperlink r:id="rId245" ref="D119"/>
-    <hyperlink r:id="rId246" ref="E119"/>
-    <hyperlink r:id="rId247" ref="D120"/>
-    <hyperlink r:id="rId248" ref="E120"/>
-    <hyperlink r:id="rId249" ref="D121"/>
-    <hyperlink r:id="rId250" ref="E121"/>
-    <hyperlink r:id="rId251" ref="F121"/>
-    <hyperlink r:id="rId252" ref="D122"/>
-    <hyperlink r:id="rId253" ref="E122"/>
-    <hyperlink r:id="rId254" ref="D123"/>
-    <hyperlink r:id="rId255" ref="E123"/>
-    <hyperlink r:id="rId256" ref="F123"/>
-    <hyperlink r:id="rId257" ref="D124"/>
-    <hyperlink r:id="rId258" ref="E124"/>
-    <hyperlink r:id="rId259" ref="D125"/>
-    <hyperlink r:id="rId260" ref="E125"/>
-    <hyperlink r:id="rId261" ref="D126"/>
-    <hyperlink r:id="rId262" ref="E126"/>
+    <hyperlink r:id="rId206" ref="D96"/>
+    <hyperlink r:id="rId207" ref="E96"/>
+    <hyperlink r:id="rId208" ref="F96"/>
+    <hyperlink r:id="rId209" ref="D97"/>
+    <hyperlink r:id="rId210" ref="E97"/>
+    <hyperlink r:id="rId211" ref="D98"/>
+    <hyperlink r:id="rId212" ref="E98"/>
+    <hyperlink r:id="rId213" ref="C99"/>
+    <hyperlink r:id="rId214" ref="D99"/>
+    <hyperlink r:id="rId215" ref="E99"/>
+    <hyperlink r:id="rId216" ref="F99"/>
+    <hyperlink r:id="rId217" ref="C100"/>
+    <hyperlink r:id="rId218" ref="D100"/>
+    <hyperlink r:id="rId219" ref="E100"/>
+    <hyperlink r:id="rId220" ref="F100"/>
+    <hyperlink r:id="rId221" ref="D101"/>
+    <hyperlink r:id="rId222" ref="E101"/>
+    <hyperlink r:id="rId223" ref="C102"/>
+    <hyperlink r:id="rId224" ref="D102"/>
+    <hyperlink r:id="rId225" ref="E102"/>
+    <hyperlink r:id="rId226" ref="D105"/>
+    <hyperlink r:id="rId227" ref="E105"/>
+    <hyperlink r:id="rId228" ref="D107"/>
+    <hyperlink r:id="rId229" ref="D108"/>
+    <hyperlink r:id="rId230" ref="E108"/>
+    <hyperlink r:id="rId231" ref="D109"/>
+    <hyperlink r:id="rId232" ref="D110"/>
+    <hyperlink r:id="rId233" ref="E110"/>
+    <hyperlink r:id="rId234" ref="F110"/>
+    <hyperlink r:id="rId235" ref="C111"/>
+    <hyperlink r:id="rId236" ref="D111"/>
+    <hyperlink r:id="rId237" ref="E111"/>
+    <hyperlink r:id="rId238" ref="D112"/>
+    <hyperlink r:id="rId239" ref="E112"/>
+    <hyperlink r:id="rId240" ref="F112"/>
+    <hyperlink r:id="rId241" ref="D114"/>
+    <hyperlink r:id="rId242" ref="D115"/>
+    <hyperlink r:id="rId243" ref="E115"/>
+    <hyperlink r:id="rId244" ref="D116"/>
+    <hyperlink r:id="rId245" ref="D117"/>
+    <hyperlink r:id="rId246" ref="D118"/>
+    <hyperlink r:id="rId247" ref="E118"/>
+    <hyperlink r:id="rId248" ref="D119"/>
+    <hyperlink r:id="rId249" ref="E119"/>
+    <hyperlink r:id="rId250" ref="D120"/>
+    <hyperlink r:id="rId251" ref="E120"/>
+    <hyperlink r:id="rId252" ref="D121"/>
+    <hyperlink r:id="rId253" ref="E121"/>
+    <hyperlink r:id="rId254" ref="D122"/>
+    <hyperlink r:id="rId255" ref="E122"/>
+    <hyperlink r:id="rId256" ref="D123"/>
+    <hyperlink r:id="rId257" ref="E123"/>
+    <hyperlink r:id="rId258" ref="D124"/>
+    <hyperlink r:id="rId259" ref="E124"/>
+    <hyperlink r:id="rId260" ref="D125"/>
+    <hyperlink r:id="rId261" ref="E125"/>
+    <hyperlink r:id="rId262" ref="F125"/>
+    <hyperlink r:id="rId263" ref="D126"/>
+    <hyperlink r:id="rId264" ref="E126"/>
+    <hyperlink r:id="rId265" ref="D127"/>
+    <hyperlink r:id="rId266" ref="E127"/>
+    <hyperlink r:id="rId267" ref="F127"/>
+    <hyperlink r:id="rId268" ref="D128"/>
+    <hyperlink r:id="rId269" ref="E128"/>
+    <hyperlink r:id="rId270" ref="D129"/>
+    <hyperlink r:id="rId271" ref="E129"/>
+    <hyperlink r:id="rId272" ref="D130"/>
+    <hyperlink r:id="rId273" ref="E130"/>
   </hyperlinks>
-  <drawing r:id="rId263"/>
+  <drawing r:id="rId274"/>
 </worksheet>
 </file>
 
@@ -14660,7 +14809,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="69" t="s">
-        <v>487</v>
+        <v>505</v>
       </c>
       <c r="G1" s="72"/>
       <c r="H1" s="72"/>
@@ -14685,27 +14834,27 @@
     </row>
     <row r="2">
       <c r="A2" s="73" t="s">
-        <v>488</v>
+        <v>506</v>
       </c>
       <c r="B2" s="74">
         <v>3.0</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>489</v>
+        <v>507</v>
       </c>
       <c r="D2" s="76" t="s">
-        <v>490</v>
+        <v>508</v>
       </c>
       <c r="E2" s="77" t="s">
-        <v>491</v>
+        <v>509</v>
       </c>
       <c r="F2" s="74" t="s">
-        <v>492</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="73" t="s">
-        <v>493</v>
+        <v>511</v>
       </c>
       <c r="B3" s="78">
         <v>45353.0</v>
@@ -14714,16 +14863,16 @@
         <v>9</v>
       </c>
       <c r="D3" s="77" t="s">
-        <v>494</v>
+        <v>512</v>
       </c>
       <c r="E3" s="76" t="s">
-        <v>495</v>
+        <v>513</v>
       </c>
       <c r="F3" s="80"/>
     </row>
     <row r="4">
       <c r="A4" s="73" t="s">
-        <v>496</v>
+        <v>514</v>
       </c>
       <c r="B4" s="74">
         <v>3.0</v>
@@ -14732,16 +14881,16 @@
         <v>9</v>
       </c>
       <c r="D4" s="76" t="s">
-        <v>497</v>
+        <v>515</v>
       </c>
       <c r="E4" s="76" t="s">
-        <v>498</v>
+        <v>516</v>
       </c>
       <c r="F4" s="80"/>
     </row>
     <row r="5">
       <c r="A5" s="73" t="s">
-        <v>499</v>
+        <v>517</v>
       </c>
       <c r="B5" s="74">
         <v>3.0</v>
@@ -14750,38 +14899,38 @@
         <v>9</v>
       </c>
       <c r="D5" s="76" t="s">
-        <v>500</v>
+        <v>518</v>
       </c>
       <c r="E5" s="81" t="s">
         <v>30</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>501</v>
+        <v>519</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="73" t="s">
-        <v>502</v>
+        <v>520</v>
       </c>
       <c r="B6" s="74">
         <v>3.0</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>503</v>
+        <v>521</v>
       </c>
       <c r="D6" s="77" t="s">
-        <v>504</v>
+        <v>522</v>
       </c>
       <c r="E6" s="77" t="s">
-        <v>505</v>
+        <v>523</v>
       </c>
       <c r="F6" s="74" t="s">
-        <v>506</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="73" t="s">
-        <v>507</v>
+        <v>525</v>
       </c>
       <c r="B7" s="74">
         <v>3.0</v>
@@ -14790,13 +14939,13 @@
         <v>9</v>
       </c>
       <c r="D7" s="76" t="s">
-        <v>508</v>
+        <v>526</v>
       </c>
       <c r="E7" s="76" t="s">
-        <v>509</v>
+        <v>527</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>510</v>
+        <v>528</v>
       </c>
     </row>
     <row r="8">
@@ -22779,22 +22928,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="84" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>512</v>
+        <v>530</v>
       </c>
       <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>513</v>
+        <v>531</v>
       </c>
       <c r="E1" s="71" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="69" t="s">
-        <v>514</v>
+        <v>532</v>
       </c>
       <c r="G1" s="72"/>
       <c r="H1" s="72"/>
@@ -22819,22 +22968,22 @@
     </row>
     <row r="2">
       <c r="A2" s="85" t="s">
-        <v>515</v>
+        <v>533</v>
       </c>
       <c r="B2" s="85" t="s">
-        <v>516</v>
+        <v>534</v>
       </c>
       <c r="C2" s="85" t="s">
         <v>55</v>
       </c>
       <c r="D2" s="85" t="s">
-        <v>517</v>
+        <v>535</v>
       </c>
       <c r="E2" s="86" t="s">
-        <v>518</v>
+        <v>536</v>
       </c>
       <c r="F2" s="85" t="s">
-        <v>519</v>
+        <v>537</v>
       </c>
       <c r="G2" s="87"/>
       <c r="H2" s="87"/>
@@ -23027,7 +23176,7 @@
     </row>
     <row r="9">
       <c r="A9" s="85" t="s">
-        <v>520</v>
+        <v>538</v>
       </c>
       <c r="B9" s="87"/>
       <c r="C9" s="87"/>
@@ -23057,7 +23206,7 @@
     </row>
     <row r="10">
       <c r="A10" s="89" t="s">
-        <v>521</v>
+        <v>539</v>
       </c>
       <c r="B10" s="87"/>
       <c r="C10" s="87"/>
@@ -26606,75 +26755,75 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="84" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>512</v>
+        <v>530</v>
       </c>
       <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>513</v>
+        <v>531</v>
       </c>
       <c r="E1" s="71" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="69" t="s">
-        <v>514</v>
+        <v>532</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="91" t="s">
-        <v>522</v>
+        <v>540</v>
       </c>
       <c r="B2" s="92"/>
       <c r="C2" s="91" t="s">
-        <v>523</v>
+        <v>541</v>
       </c>
       <c r="D2" s="93">
         <v>45746.0</v>
       </c>
       <c r="E2" s="94" t="s">
-        <v>524</v>
+        <v>542</v>
       </c>
       <c r="F2" s="95" t="s">
-        <v>525</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="91" t="s">
-        <v>526</v>
+        <v>544</v>
       </c>
       <c r="B3" s="96">
         <v>4.0</v>
       </c>
       <c r="C3" s="95" t="s">
-        <v>527</v>
+        <v>545</v>
       </c>
       <c r="D3" s="93">
         <v>45899.0</v>
       </c>
       <c r="E3" s="94" t="s">
-        <v>528</v>
+        <v>546</v>
       </c>
       <c r="F3" s="91" t="s">
-        <v>529</v>
+        <v>547</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="91" t="s">
-        <v>530</v>
+        <v>548</v>
       </c>
       <c r="B4" s="92"/>
       <c r="D4" s="93">
         <v>45884.0</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>531</v>
+        <v>549</v>
       </c>
       <c r="F4" s="95" t="s">
-        <v>532</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5">
@@ -30691,10 +30840,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>533</v>
+        <v>551</v>
       </c>
       <c r="B1" s="69" t="s">
-        <v>534</v>
+        <v>552</v>
       </c>
       <c r="C1" s="97" t="s">
         <v>3</v>
@@ -30727,89 +30876,89 @@
     </row>
     <row r="2">
       <c r="A2" s="99" t="s">
-        <v>535</v>
+        <v>553</v>
       </c>
       <c r="B2" s="96" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="100" t="s">
-        <v>536</v>
+        <v>554</v>
       </c>
       <c r="D2" s="100"/>
       <c r="E2" s="101"/>
     </row>
     <row r="3">
       <c r="A3" s="99" t="s">
-        <v>537</v>
+        <v>555</v>
       </c>
       <c r="B3" s="96" t="s">
-        <v>538</v>
+        <v>556</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>539</v>
+        <v>557</v>
       </c>
       <c r="D3" s="100"/>
       <c r="E3" s="101"/>
     </row>
     <row r="4">
       <c r="A4" s="99" t="s">
-        <v>540</v>
+        <v>558</v>
       </c>
       <c r="B4" s="96">
         <v>2024.0</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>541</v>
+        <v>559</v>
       </c>
       <c r="D4" s="100"/>
       <c r="E4" s="101"/>
     </row>
     <row r="5">
       <c r="A5" s="99" t="s">
-        <v>542</v>
+        <v>560</v>
       </c>
       <c r="B5" s="96" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>543</v>
+        <v>561</v>
       </c>
       <c r="D5" s="100"/>
       <c r="E5" s="101"/>
     </row>
     <row r="6">
       <c r="A6" s="99" t="s">
-        <v>544</v>
+        <v>562</v>
       </c>
       <c r="B6" s="96">
         <v>2025.0</v>
       </c>
       <c r="C6" s="100" t="s">
-        <v>545</v>
+        <v>563</v>
       </c>
       <c r="D6" s="100"/>
       <c r="E6" s="101"/>
     </row>
     <row r="7">
       <c r="A7" s="99" t="s">
-        <v>546</v>
+        <v>564</v>
       </c>
       <c r="B7" s="96" t="s">
-        <v>547</v>
+        <v>565</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>548</v>
+        <v>566</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="102" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="B8" s="96">
         <v>2025.0</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>550</v>
+        <v>568</v>
       </c>
     </row>
     <row r="9">
@@ -34810,82 +34959,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="104" t="s">
-        <v>551</v>
+        <v>569</v>
       </c>
       <c r="B1" s="104" t="s">
-        <v>552</v>
+        <v>570</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="105" t="s">
-        <v>553</v>
+        <v>571</v>
       </c>
       <c r="B2" s="105" t="s">
-        <v>554</v>
+        <v>572</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="105" t="s">
-        <v>555</v>
+        <v>573</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>556</v>
+        <v>574</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="105" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="105" t="s">
-        <v>559</v>
+        <v>577</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>560</v>
+        <v>578</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="105" t="s">
-        <v>561</v>
+        <v>579</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>562</v>
+        <v>580</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="105" t="s">
-        <v>563</v>
+        <v>581</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>564</v>
+        <v>582</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="105" t="s">
-        <v>565</v>
+        <v>583</v>
       </c>
       <c r="B8" s="105" t="s">
-        <v>566</v>
+        <v>584</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="105" t="s">
-        <v>567</v>
+        <v>585</v>
       </c>
       <c r="B9" s="105" t="s">
-        <v>568</v>
+        <v>586</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="105" t="s">
-        <v>569</v>
+        <v>587</v>
       </c>
       <c r="B10" s="105" t="s">
-        <v>570</v>
+        <v>588</v>
       </c>
     </row>
     <row r="11">

</xml_diff>